<commit_message>
model selection for cmac
</commit_message>
<xml_diff>
--- a/intermediate_data/ladybeetle_model_selection_results.xlsx
+++ b/intermediate_data/ladybeetle_model_selection_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cbahlai\Dropbox\Active Projects\Ohio_ladybeetles\intermediate_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81A82ABC-0CBE-48B5-B8FB-A609B1830AF5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB2D372B-D658-4232-AD30-0F426CE20639}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-1650" windowWidth="29040" windowHeight="15840" xr2:uid="{6C3B7B1D-1C13-4467-BFB9-A32EE3A2C408}"/>
   </bookViews>
@@ -31,14 +31,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="18">
   <si>
     <t>Target Species</t>
   </si>
   <si>
-    <t>Linear sampling effect</t>
-  </si>
-  <si>
     <t>Spatial smooth</t>
   </si>
   <si>
@@ -51,9 +48,6 @@
     <t>Human density</t>
   </si>
   <si>
-    <t>Aphidopagous</t>
-  </si>
-  <si>
     <t>C7</t>
   </si>
   <si>
@@ -63,9 +57,6 @@
     <t>Deviance explained</t>
   </si>
   <si>
-    <t>GCV</t>
-  </si>
-  <si>
     <t>AIC</t>
   </si>
   <si>
@@ -75,13 +66,25 @@
     <t>X</t>
   </si>
   <si>
-    <t>Forest, Developed</t>
-  </si>
-  <si>
     <t>Agriculture, Forest, Developed</t>
   </si>
   <si>
-    <t>Developed</t>
+    <t>Totalinvasive</t>
+  </si>
+  <si>
+    <t>Offset (sampling)</t>
+  </si>
+  <si>
+    <t>Adj R2</t>
+  </si>
+  <si>
+    <t>Agriculture, Forest</t>
+  </si>
+  <si>
+    <t>Forest</t>
+  </si>
+  <si>
+    <t>Final model</t>
   </si>
 </sst>
 </file>
@@ -447,13 +450,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF59FA38-E72D-4E06-86CB-265EAD803A1A}">
-  <dimension ref="A1:L22"/>
+  <dimension ref="A1:N19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomRight" activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -465,245 +468,311 @@
     <col min="5" max="5" width="17.453125" style="2" customWidth="1"/>
     <col min="6" max="6" width="18" style="2" customWidth="1"/>
     <col min="7" max="7" width="14.08984375" style="2" customWidth="1"/>
-    <col min="8" max="9" width="8.7265625" style="2"/>
+    <col min="8" max="8" width="8.7265625" style="2"/>
+    <col min="9" max="9" width="10.6328125" style="2" customWidth="1"/>
     <col min="10" max="10" width="17.6328125" style="2" customWidth="1"/>
-    <col min="11" max="12" width="8.7265625" style="2"/>
+    <col min="11" max="11" width="12.1796875" style="2" customWidth="1"/>
+    <col min="12" max="13" width="8.7265625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="J1" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="L1" s="1" t="str">
+        <f>"-REML"</f>
+        <v>-REML</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="N1" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="1" t="s">
+      <c r="B2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J2" s="2">
+        <v>0.39100000000000001</v>
+      </c>
+      <c r="K2" s="2">
+        <v>10.9</v>
+      </c>
+      <c r="L2" s="2">
+        <v>807.7</v>
+      </c>
+      <c r="M2" s="2">
+        <v>1608.2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J3" s="2">
+        <v>0.38100000000000001</v>
+      </c>
+      <c r="K3" s="2">
+        <v>21.9</v>
+      </c>
+      <c r="L3" s="2">
+        <v>795.63</v>
+      </c>
+      <c r="M3" s="2">
+        <v>1585.6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" ht="29" x14ac:dyDescent="0.35">
+      <c r="B4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J2" s="2">
-        <v>32.6</v>
-      </c>
-      <c r="K2" s="2">
-        <v>7.7439</v>
-      </c>
-      <c r="L2" s="2">
-        <v>5160.1000000000004</v>
-      </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J3" s="2">
-        <v>33.799999999999997</v>
-      </c>
-      <c r="K3" s="2">
-        <v>7.7031000000000001</v>
-      </c>
-      <c r="L3" s="2">
-        <v>5154.3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:12" ht="29" x14ac:dyDescent="0.35">
-      <c r="B4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J4" s="2">
+        <v>0.44400000000000001</v>
+      </c>
+      <c r="K4" s="2">
+        <v>4.95</v>
+      </c>
+      <c r="L4" s="2">
+        <v>819</v>
+      </c>
+      <c r="M4" s="2">
+        <v>1636.3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="29" x14ac:dyDescent="0.35">
+      <c r="B5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J5" s="2">
+        <v>0.55700000000000005</v>
+      </c>
+      <c r="K5" s="2">
+        <v>7.4</v>
+      </c>
+      <c r="L5" s="2">
+        <v>811.83</v>
+      </c>
+      <c r="M5" s="2">
+        <v>1620.9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="F4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J4" s="2">
-        <v>50.6</v>
-      </c>
-      <c r="K4" s="2">
-        <v>5.7670000000000003</v>
-      </c>
-      <c r="L4" s="2">
-        <v>4793.7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J5" s="2">
-        <v>50.6</v>
-      </c>
-      <c r="K5" s="2">
-        <v>5.7557999999999998</v>
-      </c>
-      <c r="L5" s="2">
-        <v>4791.7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E6" s="2" t="s">
+      <c r="F6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J6" s="2">
+        <v>0.55800000000000005</v>
+      </c>
+      <c r="K6" s="2">
+        <v>7.24</v>
+      </c>
+      <c r="L6" s="2">
+        <v>811.46</v>
+      </c>
+      <c r="M6" s="2">
+        <v>1617.7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J7" s="2">
+        <v>0.55900000000000005</v>
+      </c>
+      <c r="K7" s="2">
+        <v>7.01</v>
+      </c>
+      <c r="L7" s="2">
+        <v>810.23</v>
+      </c>
+      <c r="M7" s="2">
+        <v>1615.3</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="F6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="J6" s="2">
-        <v>50.6</v>
-      </c>
-      <c r="K6" s="2">
-        <v>5.7487000000000004</v>
-      </c>
-      <c r="L6" s="2">
-        <v>4790.3999999999996</v>
-      </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B7" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
-      <c r="B8" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="H8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J8" s="2">
+        <v>0.54800000000000004</v>
+      </c>
+      <c r="K8" s="2">
+        <v>6.62</v>
+      </c>
+      <c r="L8" s="2">
+        <v>809.37</v>
+      </c>
+      <c r="M8" s="2">
+        <v>1613.2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B9" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
+        <v>10</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J9" s="2">
+        <v>0.57499999999999996</v>
+      </c>
+      <c r="K9" s="2">
+        <v>4.92</v>
+      </c>
+      <c r="L9" s="2">
+        <v>813.54</v>
+      </c>
+      <c r="M9" s="2">
+        <v>1624.6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B10" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B11" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B12" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B13" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B14" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B15" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B16" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="17" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B17" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B18" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="19" spans="2:2" x14ac:dyDescent="0.35">
       <c r="B19" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B20" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B21" s="2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B22" s="2" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update cmac model selection, colours on plot
</commit_message>
<xml_diff>
--- a/intermediate_data/ladybeetle_model_selection_results.xlsx
+++ b/intermediate_data/ladybeetle_model_selection_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cbahlai\Dropbox\Active Projects\Ohio_ladybeetles\intermediate_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB2D372B-D658-4232-AD30-0F426CE20639}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A86D04B1-37F9-42B4-B578-B5E0B2359EE9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-1650" windowWidth="29040" windowHeight="15840" xr2:uid="{6C3B7B1D-1C13-4467-BFB9-A32EE3A2C408}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="18">
   <si>
     <t>Target Species</t>
   </si>
@@ -456,7 +456,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J9" sqref="J9"/>
+      <selection pane="bottomRight" activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -701,6 +701,9 @@
       <c r="M8" s="2">
         <v>1613.2</v>
       </c>
+      <c r="N8" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B9" s="2" t="s">

</xml_diff>

<commit_message>
Update model selection and plots
</commit_message>
<xml_diff>
--- a/intermediate_data/ladybeetle_model_selection_results.xlsx
+++ b/intermediate_data/ladybeetle_model_selection_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cbahlai\Dropbox\Active Projects\Ohio_ladybeetles\intermediate_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A86D04B1-37F9-42B4-B578-B5E0B2359EE9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F35D681-A04F-4197-93FE-3E63D3D417D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-1650" windowWidth="29040" windowHeight="15840" xr2:uid="{6C3B7B1D-1C13-4467-BFB9-A32EE3A2C408}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="23">
   <si>
     <t>Target Species</t>
   </si>
@@ -85,6 +85,21 @@
   </si>
   <si>
     <t>Final model</t>
+  </si>
+  <si>
+    <t>C9</t>
+  </si>
+  <si>
+    <t>Agriculture</t>
+  </si>
+  <si>
+    <t>ABI</t>
+  </si>
+  <si>
+    <t>Agriculture, Developed</t>
+  </si>
+  <si>
+    <t>Developed</t>
   </si>
 </sst>
 </file>
@@ -450,13 +465,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF59FA38-E72D-4E06-86CB-265EAD803A1A}">
-  <dimension ref="A1:N19"/>
+  <dimension ref="A1:N25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B18" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N9" sqref="N9"/>
+      <selection pane="bottomRight" activeCell="N32" sqref="N32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -728,54 +743,353 @@
         <v>1624.6</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="B10" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A11" s="2" t="s">
+        <v>18</v>
+      </c>
       <c r="B11" s="2" t="s">
         <v>10</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J11" s="2">
+        <v>0.30099999999999999</v>
+      </c>
+      <c r="K11" s="2">
+        <v>1.85</v>
+      </c>
+      <c r="L11" s="2">
+        <v>221.25</v>
+      </c>
+      <c r="M11" s="2">
+        <v>445.4</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B12" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="C12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J12" s="2">
+        <v>0.32800000000000001</v>
+      </c>
+      <c r="K12" s="2">
+        <v>7.92</v>
+      </c>
+      <c r="L12" s="2">
+        <v>217.61</v>
+      </c>
+      <c r="M12" s="2">
+        <v>447.3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="B13" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="E13" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J13" s="2">
+        <v>0.189</v>
+      </c>
+      <c r="K13" s="2">
+        <v>14.3</v>
+      </c>
+      <c r="L13" s="2">
+        <v>207.68</v>
+      </c>
+      <c r="M13" s="2">
+        <v>424.3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" ht="29" x14ac:dyDescent="0.35">
       <c r="B14" s="2" t="s">
         <v>10</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J14" s="2">
+        <v>0.184</v>
+      </c>
+      <c r="K14" s="2">
+        <v>11.4</v>
+      </c>
+      <c r="L14" s="2">
+        <v>209.81</v>
+      </c>
+      <c r="M14" s="2">
+        <v>429.36</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B15" s="2" t="s">
         <v>10</v>
       </c>
+      <c r="E15" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J15" s="2">
+        <v>0.20100000000000001</v>
+      </c>
+      <c r="K15" s="2">
+        <v>13.7</v>
+      </c>
+      <c r="L15" s="2">
+        <v>208.9</v>
+      </c>
+      <c r="M15" s="2">
+        <v>422.7</v>
+      </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B16" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="E16" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J16" s="2">
+        <v>0.28299999999999997</v>
+      </c>
+      <c r="K16" s="2">
+        <v>11.5</v>
+      </c>
+      <c r="L16" s="2">
+        <v>210.97</v>
+      </c>
+      <c r="M16" s="2">
+        <v>423.4</v>
+      </c>
+      <c r="N16" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
       <c r="B17" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.35">
-      <c r="B18" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="F17" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J17" s="2">
+        <v>0.29699999999999999</v>
+      </c>
+      <c r="K17" s="2">
+        <v>8.67</v>
+      </c>
+      <c r="L17" s="2">
+        <v>217.3</v>
+      </c>
+      <c r="M17" s="2">
+        <v>435.8</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A19" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="B19" s="2" t="s">
         <v>10</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J19" s="2">
+        <v>0.46</v>
+      </c>
+      <c r="K19" s="2">
+        <v>10.5</v>
+      </c>
+      <c r="L19" s="2">
+        <v>328.2</v>
+      </c>
+      <c r="M19" s="2">
+        <v>655.9</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B20" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J20" s="2">
+        <v>0.53800000000000003</v>
+      </c>
+      <c r="K20" s="2">
+        <v>21</v>
+      </c>
+      <c r="L20" s="2">
+        <v>316.39</v>
+      </c>
+      <c r="M20" s="2">
+        <v>638.79999999999995</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" ht="29" x14ac:dyDescent="0.35">
+      <c r="B21" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J21" s="2">
+        <v>0.54400000000000004</v>
+      </c>
+      <c r="K21" s="2">
+        <v>14.6</v>
+      </c>
+      <c r="L21" s="2">
+        <v>312.3</v>
+      </c>
+      <c r="M21" s="2">
+        <v>627.4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:14" ht="29" x14ac:dyDescent="0.35">
+      <c r="B22" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J22" s="2">
+        <v>0.53900000000000003</v>
+      </c>
+      <c r="K22" s="2">
+        <v>12.2</v>
+      </c>
+      <c r="L22" s="2">
+        <v>316.12</v>
+      </c>
+      <c r="M22" s="2">
+        <v>634.79999999999995</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" ht="29" x14ac:dyDescent="0.35">
+      <c r="B23" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J23" s="2">
+        <v>0.54100000000000004</v>
+      </c>
+      <c r="K23" s="2">
+        <v>14</v>
+      </c>
+      <c r="L23" s="2">
+        <v>313.74</v>
+      </c>
+      <c r="M23" s="2">
+        <v>625.9</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" ht="29" x14ac:dyDescent="0.35">
+      <c r="B24" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J24" s="2">
+        <v>0.53900000000000003</v>
+      </c>
+      <c r="K24" s="2">
+        <v>13.1</v>
+      </c>
+      <c r="L24" s="2">
+        <v>313.38</v>
+      </c>
+      <c r="M24" s="2">
+        <v>625.29999999999995</v>
+      </c>
+      <c r="N24" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B25" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J25" s="2">
+        <v>0.50600000000000001</v>
+      </c>
+      <c r="K25" s="2">
+        <v>9.7200000000000006</v>
+      </c>
+      <c r="L25" s="2">
+        <v>316.27999999999997</v>
+      </c>
+      <c r="M25" s="2">
+        <v>631.4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add Hcon analysis and figures
</commit_message>
<xml_diff>
--- a/intermediate_data/ladybeetle_model_selection_results.xlsx
+++ b/intermediate_data/ladybeetle_model_selection_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cbahlai\Dropbox\Active Projects\Ohio_ladybeetles\intermediate_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F35D681-A04F-4197-93FE-3E63D3D417D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55D819A8-2B27-4C7F-BE40-7B14373AD1F7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-1650" windowWidth="29040" windowHeight="15840" xr2:uid="{6C3B7B1D-1C13-4467-BFB9-A32EE3A2C408}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="25">
   <si>
     <t>Target Species</t>
   </si>
@@ -100,6 +100,12 @@
   </si>
   <si>
     <t>Developed</t>
+  </si>
+  <si>
+    <t>HCON</t>
+  </si>
+  <si>
+    <t>Forest, Developed</t>
   </si>
 </sst>
 </file>
@@ -465,13 +471,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF59FA38-E72D-4E06-86CB-265EAD803A1A}">
-  <dimension ref="A1:N25"/>
+  <dimension ref="A1:N34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B18" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B26" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="N32" sqref="N32"/>
+      <selection pane="bottomRight" activeCell="L37" sqref="L37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1092,6 +1098,175 @@
         <v>631.4</v>
       </c>
     </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A27" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J27" s="2">
+        <v>0.39100000000000001</v>
+      </c>
+      <c r="K27" s="2">
+        <v>10.9</v>
+      </c>
+      <c r="L27" s="2">
+        <v>807.7</v>
+      </c>
+      <c r="M27" s="2">
+        <v>922.1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B28" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J28" s="2">
+        <v>0.51400000000000001</v>
+      </c>
+      <c r="K28" s="2">
+        <v>32</v>
+      </c>
+      <c r="L28" s="2">
+        <v>450.46</v>
+      </c>
+      <c r="M28" s="2">
+        <v>885.6</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" ht="29" x14ac:dyDescent="0.35">
+      <c r="B29" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J29" s="2">
+        <v>0.48799999999999999</v>
+      </c>
+      <c r="K29" s="2">
+        <v>20.6</v>
+      </c>
+      <c r="L29" s="2">
+        <v>444.37</v>
+      </c>
+      <c r="M29" s="2">
+        <v>881.5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:14" ht="29" x14ac:dyDescent="0.35">
+      <c r="B30" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J30" s="2">
+        <v>0.308</v>
+      </c>
+      <c r="K30" s="2">
+        <v>23.1</v>
+      </c>
+      <c r="L30" s="2">
+        <v>439.3</v>
+      </c>
+      <c r="M30" s="2">
+        <v>870.9</v>
+      </c>
+    </row>
+    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B31" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="J31" s="2">
+        <v>0.255</v>
+      </c>
+      <c r="K31" s="2">
+        <v>22.3</v>
+      </c>
+      <c r="L31" s="2">
+        <v>440.66</v>
+      </c>
+      <c r="M31" s="2">
+        <v>870.4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="B32" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I32" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="33" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B33" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I33" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="2:9" x14ac:dyDescent="0.35">
+      <c r="B34" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="I34" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
model selection stats update
</commit_message>
<xml_diff>
--- a/intermediate_data/ladybeetle_model_selection_results.xlsx
+++ b/intermediate_data/ladybeetle_model_selection_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cbahlai\Dropbox\Active Projects\Ohio_ladybeetles\intermediate_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7C7002D-4224-44B3-949E-B2257053CD8B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F478E87-E196-47D5-81BC-356DB7BCEECA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-1650" windowWidth="29040" windowHeight="15840" xr2:uid="{6C3B7B1D-1C13-4467-BFB9-A32EE3A2C408}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="36">
   <si>
     <t>Target Species</t>
   </si>
@@ -517,10 +517,10 @@
   <dimension ref="A1:S75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B14" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="Q33" sqref="Q33"/>
+      <selection pane="bottomRight" activeCell="T38" sqref="T38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1520,52 +1520,277 @@
         <v>33</v>
       </c>
     </row>
-    <row r="33" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:18" ht="29" x14ac:dyDescent="0.35">
       <c r="B33" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="34" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="E33" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I33" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K33" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="N33" s="2">
+        <v>0.36099999999999999</v>
+      </c>
+      <c r="O33" s="2">
+        <v>24.8</v>
+      </c>
+      <c r="P33" s="2">
+        <v>304.31</v>
+      </c>
+      <c r="Q33" s="2">
+        <v>616.79999999999995</v>
+      </c>
+    </row>
+    <row r="34" spans="1:18" ht="29" x14ac:dyDescent="0.35">
       <c r="B34" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="35" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="E34" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I34" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K34" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L34" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M34" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="N34" s="2">
+        <v>0.374</v>
+      </c>
+      <c r="O34" s="2">
+        <v>24.9</v>
+      </c>
+      <c r="P34" s="2">
+        <v>305.3</v>
+      </c>
+      <c r="Q34" s="2">
+        <v>618.5</v>
+      </c>
+    </row>
+    <row r="35" spans="1:18" ht="29" x14ac:dyDescent="0.35">
       <c r="B35" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="36" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="E35" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I35" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K35" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="N35" s="2">
+        <v>0.34200000000000003</v>
+      </c>
+      <c r="O35" s="2">
+        <v>24.6</v>
+      </c>
+      <c r="P35" s="2">
+        <v>305.60000000000002</v>
+      </c>
+      <c r="Q35" s="2">
+        <v>614.23</v>
+      </c>
+    </row>
+    <row r="36" spans="1:18" ht="29" x14ac:dyDescent="0.35">
       <c r="B36" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="37" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="E36" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H36" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I36" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K36" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="N36" s="2">
+        <v>0.313</v>
+      </c>
+      <c r="O36" s="2">
+        <v>24.2</v>
+      </c>
+      <c r="P36" s="2">
+        <v>307.11</v>
+      </c>
+      <c r="Q36" s="2">
+        <v>612.19000000000005</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" ht="29" x14ac:dyDescent="0.35">
       <c r="B37" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="38" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="F37" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I37" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K37" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="N37" s="2">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="O37" s="2">
+        <v>23.5</v>
+      </c>
+      <c r="P37" s="2">
+        <v>306.24</v>
+      </c>
+      <c r="Q37" s="2">
+        <v>610.99</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" ht="29" x14ac:dyDescent="0.35">
       <c r="B38" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="39" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="F38" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="I38" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K38" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="N38" s="2">
+        <v>0.35699999999999998</v>
+      </c>
+      <c r="O38" s="2">
+        <v>22</v>
+      </c>
+      <c r="P38" s="2">
+        <v>306.17</v>
+      </c>
+      <c r="Q38" s="2">
+        <v>611.6</v>
+      </c>
+    </row>
+    <row r="39" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B39" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="40" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="F39" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I39" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K39" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="N39" s="2">
+        <v>0.35</v>
+      </c>
+      <c r="O39" s="2">
+        <v>21.5</v>
+      </c>
+      <c r="P39" s="2">
+        <v>305.64999999999998</v>
+      </c>
+      <c r="Q39" s="2">
+        <v>609.57000000000005</v>
+      </c>
+      <c r="R39" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B40" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="41" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="H40" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I40" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K40" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="N40" s="2">
+        <v>0.38500000000000001</v>
+      </c>
+      <c r="O40" s="2">
+        <v>17.3</v>
+      </c>
+      <c r="P40" s="2">
+        <v>307.92</v>
+      </c>
+      <c r="Q40" s="2">
+        <v>616.82000000000005</v>
+      </c>
+    </row>
+    <row r="41" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B41" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="43" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A43" s="3" t="s">
         <v>21</v>
       </c>
@@ -1598,7 +1823,7 @@
         <v>922.1</v>
       </c>
     </row>
-    <row r="44" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A44" s="3"/>
       <c r="B44" s="3" t="s">
         <v>8</v>
@@ -1631,7 +1856,7 @@
         <v>885.6</v>
       </c>
     </row>
-    <row r="45" spans="1:17" ht="29" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:18" ht="29" x14ac:dyDescent="0.35">
       <c r="B45" s="2" t="s">
         <v>8</v>
       </c>
@@ -1654,7 +1879,7 @@
         <v>881.5</v>
       </c>
     </row>
-    <row r="46" spans="1:17" ht="29" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:18" ht="29" x14ac:dyDescent="0.35">
       <c r="B46" s="2" t="s">
         <v>8</v>
       </c>
@@ -1680,7 +1905,7 @@
         <v>870.9</v>
       </c>
     </row>
-    <row r="47" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B47" s="2" t="s">
         <v>8</v>
       </c>
@@ -1706,7 +1931,7 @@
         <v>870.4</v>
       </c>
     </row>
-    <row r="48" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B48" s="2" t="s">
         <v>8</v>
       </c>

</xml_diff>

<commit_message>
complete hcon and cstig model selections
</commit_message>
<xml_diff>
--- a/intermediate_data/ladybeetle_model_selection_results.xlsx
+++ b/intermediate_data/ladybeetle_model_selection_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cbahlai\Dropbox\Active Projects\Ohio_ladybeetles\intermediate_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4F478E87-E196-47D5-81BC-356DB7BCEECA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CDBEB11-9A20-4870-93A7-B6F7088440A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-1650" windowWidth="29040" windowHeight="15840" xr2:uid="{6C3B7B1D-1C13-4467-BFB9-A32EE3A2C408}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="318" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="36">
   <si>
     <t>Target Species</t>
   </si>
@@ -99,46 +99,46 @@
     <t>HCON</t>
   </si>
   <si>
+    <t>CSTIG</t>
+  </si>
+  <si>
+    <t>Aphidophagous</t>
+  </si>
+  <si>
+    <t>HAXY</t>
+  </si>
+  <si>
+    <t>3 Decade group</t>
+  </si>
+  <si>
+    <t>Decade</t>
+  </si>
+  <si>
+    <t>Rate of landscape change</t>
+  </si>
+  <si>
+    <t>Latitude</t>
+  </si>
+  <si>
+    <t>Longitude</t>
+  </si>
+  <si>
+    <t>Invasive ratio</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t>Totalinvasive needs to be limited to k=4</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>Agriculture,  Developed</t>
+  </si>
+  <si>
     <t>Forest, Developed</t>
-  </si>
-  <si>
-    <t>CSTIG</t>
-  </si>
-  <si>
-    <t>Aphidophagous</t>
-  </si>
-  <si>
-    <t>HAXY</t>
-  </si>
-  <si>
-    <t>3 Decade group</t>
-  </si>
-  <si>
-    <t>Decade</t>
-  </si>
-  <si>
-    <t>Rate of landscape change</t>
-  </si>
-  <si>
-    <t>Latitude</t>
-  </si>
-  <si>
-    <t>Longitude</t>
-  </si>
-  <si>
-    <t>Invasive ratio</t>
-  </si>
-  <si>
-    <t>Notes</t>
-  </si>
-  <si>
-    <t>Totalinvasive needs to be limited to k=4</t>
-  </si>
-  <si>
-    <t>NA</t>
-  </si>
-  <si>
-    <t>Agriculture,  Developed</t>
   </si>
 </sst>
 </file>
@@ -514,13 +514,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF59FA38-E72D-4E06-86CB-265EAD803A1A}">
-  <dimension ref="A1:S75"/>
+  <dimension ref="A1:S83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B20" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B50" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="T38" sqref="T38"/>
+      <selection pane="bottomRight" activeCell="R67" sqref="R67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -552,28 +552,28 @@
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>27</v>
-      </c>
       <c r="F1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>10</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L1" s="1" t="s">
         <v>3</v>
@@ -598,7 +598,7 @@
         <v>15</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.35">
@@ -1135,7 +1135,7 @@
         <v>402.69</v>
       </c>
       <c r="S18" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="19" spans="1:19" ht="29" x14ac:dyDescent="0.35">
@@ -1199,7 +1199,7 @@
         <v>8</v>
       </c>
       <c r="M20" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="N20" s="2">
         <v>-0.501</v>
@@ -1324,7 +1324,7 @@
         <v>8</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I24" s="2" t="s">
         <v>14</v>
@@ -1406,80 +1406,143 @@
         <v>396.51</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="B27" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.35">
-      <c r="B28" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="30" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A30" s="3" t="s">
+    <row r="28" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A28" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B30" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C30" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
-      <c r="H30" s="3"/>
-      <c r="I30" s="3"/>
-      <c r="J30" s="3"/>
-      <c r="K30" s="3"/>
-      <c r="L30" s="3"/>
-      <c r="M30" s="3"/>
-      <c r="N30" s="3">
+      <c r="B28" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C28" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="3"/>
+      <c r="J28" s="3"/>
+      <c r="K28" s="3"/>
+      <c r="L28" s="3"/>
+      <c r="M28" s="3"/>
+      <c r="N28" s="3">
         <v>0.46</v>
       </c>
-      <c r="O30" s="3">
+      <c r="O28" s="3">
         <v>10.5</v>
       </c>
-      <c r="P30" s="3">
+      <c r="P28" s="3">
         <v>328.2</v>
       </c>
-      <c r="Q30" s="3">
+      <c r="Q28" s="3">
         <v>655.9</v>
       </c>
     </row>
-    <row r="31" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="3"/>
-      <c r="B31" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C31" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D31" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
-      <c r="I31" s="3"/>
-      <c r="J31" s="3"/>
-      <c r="K31" s="3"/>
-      <c r="L31" s="3"/>
-      <c r="M31" s="3"/>
-      <c r="N31" s="3">
+    <row r="29" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="3"/>
+      <c r="B29" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C29" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D29" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="3"/>
+      <c r="J29" s="3"/>
+      <c r="K29" s="3"/>
+      <c r="L29" s="3"/>
+      <c r="M29" s="3"/>
+      <c r="N29" s="3">
         <v>0.53800000000000003</v>
       </c>
-      <c r="O31" s="3">
+      <c r="O29" s="3">
         <v>21</v>
       </c>
-      <c r="P31" s="3">
+      <c r="P29" s="3">
         <v>316.39</v>
       </c>
-      <c r="Q31" s="3">
+      <c r="Q29" s="3">
         <v>638.79999999999995</v>
+      </c>
+    </row>
+    <row r="30" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+      <c r="B30" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="N30" s="2">
+        <v>0.39800000000000002</v>
+      </c>
+      <c r="O30" s="2">
+        <v>23.5</v>
+      </c>
+      <c r="P30" s="2">
+        <v>308.18</v>
+      </c>
+      <c r="Q30" s="2">
+        <v>621.16999999999996</v>
+      </c>
+      <c r="S30" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="31" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+      <c r="B31" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K31" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="N31" s="2">
+        <v>0.36099999999999999</v>
+      </c>
+      <c r="O31" s="2">
+        <v>24.8</v>
+      </c>
+      <c r="P31" s="2">
+        <v>304.31</v>
+      </c>
+      <c r="Q31" s="2">
+        <v>616.79999999999995</v>
       </c>
     </row>
     <row r="32" spans="1:19" ht="29" x14ac:dyDescent="0.35">
@@ -1501,23 +1564,26 @@
       <c r="I32" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="J32" s="2" t="s">
-        <v>8</v>
+      <c r="K32" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L32" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M32" s="2" t="s">
+        <v>33</v>
       </c>
       <c r="N32" s="2">
-        <v>0.39800000000000002</v>
+        <v>0.374</v>
       </c>
       <c r="O32" s="2">
-        <v>23.5</v>
+        <v>24.9</v>
       </c>
       <c r="P32" s="2">
-        <v>308.18</v>
+        <v>305.3</v>
       </c>
       <c r="Q32" s="2">
-        <v>621.16999999999996</v>
-      </c>
-      <c r="S32" t="s">
-        <v>33</v>
+        <v>618.5</v>
       </c>
     </row>
     <row r="33" spans="1:18" ht="29" x14ac:dyDescent="0.35">
@@ -1534,7 +1600,7 @@
         <v>8</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>9</v>
+        <v>34</v>
       </c>
       <c r="I33" s="2" t="s">
         <v>9</v>
@@ -1543,16 +1609,16 @@
         <v>8</v>
       </c>
       <c r="N33" s="2">
-        <v>0.36099999999999999</v>
+        <v>0.34200000000000003</v>
       </c>
       <c r="O33" s="2">
-        <v>24.8</v>
+        <v>24.6</v>
       </c>
       <c r="P33" s="2">
-        <v>304.31</v>
+        <v>305.60000000000002</v>
       </c>
       <c r="Q33" s="2">
-        <v>616.79999999999995</v>
+        <v>614.23</v>
       </c>
     </row>
     <row r="34" spans="1:18" ht="29" x14ac:dyDescent="0.35">
@@ -1569,40 +1635,31 @@
         <v>8</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>9</v>
+        <v>34</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="K34" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="L34" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="M34" s="2" t="s">
-        <v>34</v>
-      </c>
       <c r="N34" s="2">
-        <v>0.374</v>
+        <v>0.313</v>
       </c>
       <c r="O34" s="2">
-        <v>24.9</v>
+        <v>24.2</v>
       </c>
       <c r="P34" s="2">
-        <v>305.3</v>
+        <v>307.11</v>
       </c>
       <c r="Q34" s="2">
-        <v>618.5</v>
+        <v>612.19000000000005</v>
       </c>
     </row>
     <row r="35" spans="1:18" ht="29" x14ac:dyDescent="0.35">
       <c r="B35" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E35" s="2" t="s">
-        <v>8</v>
-      </c>
       <c r="F35" s="2" t="s">
         <v>8</v>
       </c>
@@ -1610,42 +1667,36 @@
         <v>8</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="K35" s="2" t="s">
         <v>8</v>
       </c>
       <c r="N35" s="2">
-        <v>0.34200000000000003</v>
+        <v>0.13500000000000001</v>
       </c>
       <c r="O35" s="2">
-        <v>24.6</v>
+        <v>23.5</v>
       </c>
       <c r="P35" s="2">
-        <v>305.60000000000002</v>
+        <v>306.24</v>
       </c>
       <c r="Q35" s="2">
-        <v>614.23</v>
+        <v>610.99</v>
       </c>
     </row>
     <row r="36" spans="1:18" ht="29" x14ac:dyDescent="0.35">
       <c r="B36" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E36" s="2" t="s">
-        <v>8</v>
-      </c>
       <c r="F36" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G36" s="2" t="s">
-        <v>8</v>
-      </c>
       <c r="H36" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="I36" s="2" t="s">
         <v>13</v>
@@ -1654,30 +1705,27 @@
         <v>8</v>
       </c>
       <c r="N36" s="2">
-        <v>0.313</v>
+        <v>0.35699999999999998</v>
       </c>
       <c r="O36" s="2">
-        <v>24.2</v>
+        <v>22</v>
       </c>
       <c r="P36" s="2">
-        <v>307.11</v>
+        <v>306.17</v>
       </c>
       <c r="Q36" s="2">
-        <v>612.19000000000005</v>
-      </c>
-    </row>
-    <row r="37" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+        <v>611.6</v>
+      </c>
+    </row>
+    <row r="37" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B37" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F37" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G37" s="2" t="s">
-        <v>8</v>
-      </c>
       <c r="H37" s="2" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="I37" s="2" t="s">
         <v>13</v>
@@ -1686,27 +1734,27 @@
         <v>8</v>
       </c>
       <c r="N37" s="2">
-        <v>0.13500000000000001</v>
+        <v>0.35</v>
       </c>
       <c r="O37" s="2">
-        <v>23.5</v>
+        <v>21.5</v>
       </c>
       <c r="P37" s="2">
-        <v>306.24</v>
+        <v>305.64999999999998</v>
       </c>
       <c r="Q37" s="2">
-        <v>610.99</v>
-      </c>
-    </row>
-    <row r="38" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+        <v>609.57000000000005</v>
+      </c>
+      <c r="R37" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="38" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B38" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F38" s="2" t="s">
-        <v>8</v>
-      </c>
       <c r="H38" s="2" t="s">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="I38" s="2" t="s">
         <v>13</v>
@@ -1715,176 +1763,221 @@
         <v>8</v>
       </c>
       <c r="N38" s="2">
-        <v>0.35699999999999998</v>
+        <v>0.38500000000000001</v>
       </c>
       <c r="O38" s="2">
-        <v>22</v>
+        <v>17.3</v>
       </c>
       <c r="P38" s="2">
-        <v>306.17</v>
+        <v>307.92</v>
       </c>
       <c r="Q38" s="2">
-        <v>611.6</v>
+        <v>616.82000000000005</v>
       </c>
     </row>
     <row r="39" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B39" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F39" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H39" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I39" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="K39" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="N39" s="2">
-        <v>0.35</v>
-      </c>
-      <c r="O39" s="2">
-        <v>21.5</v>
-      </c>
-      <c r="P39" s="2">
-        <v>305.64999999999998</v>
-      </c>
-      <c r="Q39" s="2">
-        <v>609.57000000000005</v>
-      </c>
-      <c r="R39" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="B40" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H40" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I40" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="K40" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="N40" s="2">
-        <v>0.38500000000000001</v>
-      </c>
-      <c r="O40" s="2">
-        <v>17.3</v>
-      </c>
-      <c r="P40" s="2">
-        <v>307.92</v>
-      </c>
-      <c r="Q40" s="2">
-        <v>616.82000000000005</v>
-      </c>
-    </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="B41" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="43" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A43" s="3" t="s">
+    </row>
+    <row r="41" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B43" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D43" s="3"/>
-      <c r="E43" s="3"/>
-      <c r="F43" s="3"/>
-      <c r="G43" s="3"/>
-      <c r="H43" s="3"/>
-      <c r="I43" s="3"/>
-      <c r="J43" s="3"/>
-      <c r="K43" s="3"/>
-      <c r="L43" s="3"/>
-      <c r="M43" s="3"/>
-      <c r="N43" s="3">
+      <c r="B41" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D41" s="3"/>
+      <c r="E41" s="3"/>
+      <c r="F41" s="3"/>
+      <c r="G41" s="3"/>
+      <c r="H41" s="3"/>
+      <c r="I41" s="3"/>
+      <c r="J41" s="3"/>
+      <c r="K41" s="3"/>
+      <c r="L41" s="3"/>
+      <c r="M41" s="3"/>
+      <c r="N41" s="3">
         <v>0.26900000000000002</v>
       </c>
-      <c r="O43" s="3">
+      <c r="O41" s="3">
         <v>9.86</v>
       </c>
-      <c r="P43" s="3">
+      <c r="P41" s="3">
         <v>462.17</v>
       </c>
-      <c r="Q43" s="3">
+      <c r="Q41" s="3">
         <v>922.1</v>
       </c>
     </row>
-    <row r="44" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A44" s="3"/>
-      <c r="B44" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C44" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D44" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E44" s="3"/>
-      <c r="F44" s="3"/>
-      <c r="G44" s="3"/>
-      <c r="H44" s="3"/>
-      <c r="I44" s="3"/>
-      <c r="J44" s="3"/>
-      <c r="K44" s="3"/>
-      <c r="L44" s="3"/>
-      <c r="M44" s="3"/>
-      <c r="N44" s="3">
+    <row r="42" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="3"/>
+      <c r="B42" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E42" s="3"/>
+      <c r="F42" s="3"/>
+      <c r="G42" s="3"/>
+      <c r="H42" s="3"/>
+      <c r="I42" s="3"/>
+      <c r="J42" s="3"/>
+      <c r="K42" s="3"/>
+      <c r="L42" s="3"/>
+      <c r="M42" s="3"/>
+      <c r="N42" s="3">
         <v>0.51400000000000001</v>
       </c>
-      <c r="O44" s="3">
+      <c r="O42" s="3">
         <v>32</v>
       </c>
-      <c r="P44" s="3">
+      <c r="P42" s="3">
         <v>450.46</v>
       </c>
-      <c r="Q44" s="3">
+      <c r="Q42" s="3">
         <v>885.6</v>
+      </c>
+    </row>
+    <row r="43" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+      <c r="B43" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H43" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I43" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J43" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="N43" s="2">
+        <v>0.63600000000000001</v>
+      </c>
+      <c r="O43" s="2">
+        <v>35.6</v>
+      </c>
+      <c r="P43" s="2">
+        <v>422.26</v>
+      </c>
+      <c r="Q43" s="2">
+        <v>840.36</v>
+      </c>
+    </row>
+    <row r="44" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+      <c r="B44" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H44" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I44" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K44" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="N44" s="2">
+        <v>0.64500000000000002</v>
+      </c>
+      <c r="O44" s="2">
+        <v>36.700000000000003</v>
+      </c>
+      <c r="P44" s="2">
+        <v>418.94</v>
+      </c>
+      <c r="Q44" s="2">
+        <v>836.77</v>
       </c>
     </row>
     <row r="45" spans="1:18" ht="29" x14ac:dyDescent="0.35">
       <c r="B45" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="E45" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="H45" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="J45" s="2" t="s">
+      <c r="I45" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K45" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L45" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M45" s="2" t="s">
         <v>8</v>
       </c>
       <c r="N45" s="2">
-        <v>0.48799999999999999</v>
+        <v>0.25800000000000001</v>
       </c>
       <c r="O45" s="2">
-        <v>20.6</v>
+        <v>38.5</v>
       </c>
       <c r="P45" s="2">
-        <v>444.37</v>
+        <v>415.96</v>
       </c>
       <c r="Q45" s="2">
-        <v>881.5</v>
+        <v>832.06</v>
       </c>
     </row>
     <row r="46" spans="1:18" ht="29" x14ac:dyDescent="0.35">
       <c r="B46" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="E46" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="H46" s="2" t="s">
-        <v>9</v>
+        <v>19</v>
+      </c>
+      <c r="I46" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K46" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="L46" s="2" t="s">
         <v>8</v>
@@ -1893,24 +1986,39 @@
         <v>8</v>
       </c>
       <c r="N46" s="2">
-        <v>0.308</v>
+        <v>0.30599999999999999</v>
       </c>
       <c r="O46" s="2">
-        <v>23.1</v>
+        <v>37.6</v>
       </c>
       <c r="P46" s="2">
-        <v>439.3</v>
+        <v>418.32</v>
       </c>
       <c r="Q46" s="2">
-        <v>870.9</v>
-      </c>
-    </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.35">
+        <v>832.62</v>
+      </c>
+    </row>
+    <row r="47" spans="1:18" ht="29" x14ac:dyDescent="0.35">
       <c r="B47" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="E47" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="H47" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
+      </c>
+      <c r="I47" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K47" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="L47" s="2" t="s">
         <v>8</v>
@@ -1919,25 +2027,40 @@
         <v>8</v>
       </c>
       <c r="N47" s="2">
-        <v>0.255</v>
+        <v>0.30499999999999999</v>
       </c>
       <c r="O47" s="2">
-        <v>22.3</v>
+        <v>37.200000000000003</v>
       </c>
       <c r="P47" s="2">
-        <v>440.66</v>
+        <v>417.73</v>
       </c>
       <c r="Q47" s="2">
-        <v>870.4</v>
-      </c>
-    </row>
-    <row r="48" spans="1:18" x14ac:dyDescent="0.35">
+        <v>830.9</v>
+      </c>
+    </row>
+    <row r="48" spans="1:18" ht="29" x14ac:dyDescent="0.35">
       <c r="B48" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G48" s="2" t="s">
         <v>8</v>
       </c>
       <c r="H48" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="I48" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="K48" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="L48" s="2" t="s">
         <v>8</v>
       </c>
@@ -1945,447 +2068,541 @@
         <v>8</v>
       </c>
       <c r="N48" s="2">
-        <v>0.27300000000000002</v>
+        <v>0.316</v>
       </c>
       <c r="O48" s="2">
-        <v>21.1</v>
+        <v>36.9</v>
       </c>
       <c r="P48" s="2">
-        <v>439.84</v>
+        <v>419.43</v>
       </c>
       <c r="Q48" s="2">
-        <v>870.8</v>
-      </c>
-    </row>
-    <row r="49" spans="1:18" x14ac:dyDescent="0.35">
+        <v>828.98</v>
+      </c>
+    </row>
+    <row r="49" spans="1:18" ht="29" x14ac:dyDescent="0.35">
       <c r="B49" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G49" s="2" t="s">
         <v>8</v>
       </c>
       <c r="H49" s="2" t="s">
         <v>20</v>
       </c>
+      <c r="I49" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="K49" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L49" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="M49" s="2" t="s">
         <v>8</v>
       </c>
       <c r="N49" s="2">
-        <v>0.44</v>
+        <v>0.38600000000000001</v>
       </c>
       <c r="O49" s="2">
-        <v>20.7</v>
+        <v>35.9</v>
       </c>
       <c r="P49" s="2">
-        <v>439.64</v>
+        <v>418.03</v>
       </c>
       <c r="Q49" s="2">
-        <v>870.4</v>
+        <v>827.44</v>
       </c>
       <c r="R49" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="50" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:18" ht="29" x14ac:dyDescent="0.35">
       <c r="B50" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="E50" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G50" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I50" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="K50" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L50" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="M50" s="2" t="s">
         <v>8</v>
       </c>
       <c r="N50" s="2">
-        <v>0.39800000000000002</v>
+        <v>0.27300000000000002</v>
       </c>
       <c r="O50" s="2">
-        <v>15.9</v>
+        <v>33.9</v>
       </c>
       <c r="P50" s="2">
-        <v>447.62</v>
+        <v>419.11</v>
       </c>
       <c r="Q50" s="2">
-        <v>890.6</v>
-      </c>
-    </row>
-    <row r="52" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A52" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B52" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C52" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D52" s="3"/>
-      <c r="E52" s="3"/>
-      <c r="F52" s="3"/>
-      <c r="G52" s="3"/>
-      <c r="H52" s="3"/>
-      <c r="I52" s="3"/>
-      <c r="J52" s="3"/>
-      <c r="K52" s="3"/>
-      <c r="L52" s="3"/>
-      <c r="M52" s="3"/>
-      <c r="N52" s="3">
+        <v>832.07</v>
+      </c>
+    </row>
+    <row r="55" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D55" s="3"/>
+      <c r="E55" s="3"/>
+      <c r="F55" s="3"/>
+      <c r="G55" s="3"/>
+      <c r="H55" s="3"/>
+      <c r="I55" s="3"/>
+      <c r="J55" s="3"/>
+      <c r="K55" s="3"/>
+      <c r="L55" s="3"/>
+      <c r="M55" s="3"/>
+      <c r="N55" s="3">
         <v>1.8499999999999999E-2</v>
       </c>
-      <c r="O52" s="3">
+      <c r="O55" s="3">
         <v>28.6</v>
       </c>
-      <c r="P52" s="3">
+      <c r="P55" s="3">
         <v>248.46</v>
       </c>
-      <c r="Q52" s="3">
+      <c r="Q55" s="3">
         <v>497.3</v>
       </c>
     </row>
-    <row r="53" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A53" s="3"/>
-      <c r="B53" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C53" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D53" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E53" s="3"/>
-      <c r="F53" s="3"/>
-      <c r="G53" s="3"/>
-      <c r="H53" s="3"/>
-      <c r="I53" s="3"/>
-      <c r="J53" s="3"/>
-      <c r="K53" s="3"/>
-      <c r="L53" s="3"/>
-      <c r="M53" s="3"/>
-      <c r="N53" s="3">
+    <row r="56" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A56" s="3"/>
+      <c r="B56" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E56" s="3"/>
+      <c r="F56" s="3"/>
+      <c r="G56" s="3"/>
+      <c r="H56" s="3"/>
+      <c r="I56" s="3"/>
+      <c r="J56" s="3"/>
+      <c r="K56" s="3"/>
+      <c r="L56" s="3"/>
+      <c r="M56" s="3"/>
+      <c r="N56" s="3">
         <v>2.6100000000000002E-2</v>
       </c>
-      <c r="O53" s="3">
+      <c r="O56" s="3">
         <v>30.1</v>
       </c>
-      <c r="P53" s="3">
+      <c r="P56" s="3">
         <v>242.65</v>
       </c>
-      <c r="Q53" s="3">
+      <c r="Q56" s="3">
         <v>510.23</v>
-      </c>
-    </row>
-    <row r="54" spans="1:18" ht="29" x14ac:dyDescent="0.35">
-      <c r="B54" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H54" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="J54" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="N54" s="2">
-        <v>0.186</v>
-      </c>
-      <c r="O54" s="2">
-        <v>22.2</v>
-      </c>
-      <c r="P54" s="2">
-        <v>248.77</v>
-      </c>
-      <c r="Q54" s="2">
-        <v>502.23</v>
-      </c>
-    </row>
-    <row r="55" spans="1:18" ht="29" x14ac:dyDescent="0.35">
-      <c r="B55" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H55" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="L55" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="M55" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="N55" s="2">
-        <v>0.14000000000000001</v>
-      </c>
-      <c r="O55" s="2">
-        <v>19.100000000000001</v>
-      </c>
-      <c r="P55" s="2">
-        <v>250.7</v>
-      </c>
-      <c r="Q55" s="2">
-        <v>509.04</v>
-      </c>
-    </row>
-    <row r="56" spans="1:18" ht="29" x14ac:dyDescent="0.35">
-      <c r="B56" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H56" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="J56" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="N56" s="2">
-        <v>0.14799999999999999</v>
-      </c>
-      <c r="O56" s="2">
-        <v>21.4</v>
-      </c>
-      <c r="P56" s="2">
-        <v>248.53</v>
-      </c>
-      <c r="Q56" s="2">
-        <v>501.31</v>
-      </c>
-      <c r="R56" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="57" spans="1:18" ht="29" x14ac:dyDescent="0.35">
       <c r="B57" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="E57" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G57" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="H57" s="2" t="s">
-        <v>19</v>
+        <v>9</v>
+      </c>
+      <c r="I57" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J57" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="N57" s="2">
-        <v>0.30399999999999999</v>
+        <v>0.222</v>
       </c>
       <c r="O57" s="2">
-        <v>18.100000000000001</v>
+        <v>29.5</v>
       </c>
       <c r="P57" s="2">
-        <v>253.12</v>
+        <v>242.93</v>
       </c>
       <c r="Q57" s="2">
-        <v>505.52</v>
-      </c>
-    </row>
-    <row r="58" spans="1:18" x14ac:dyDescent="0.35">
+        <v>498.99</v>
+      </c>
+    </row>
+    <row r="58" spans="1:18" ht="29" x14ac:dyDescent="0.35">
       <c r="B58" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="E58" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F58" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G58" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="H58" s="2" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="59" spans="1:18" x14ac:dyDescent="0.35">
+        <v>9</v>
+      </c>
+      <c r="I58" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K58" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="N58" s="2">
+        <v>0.34399999999999997</v>
+      </c>
+      <c r="O58" s="2">
+        <v>30.6</v>
+      </c>
+      <c r="P58" s="2">
+        <v>240.42</v>
+      </c>
+      <c r="Q58" s="2">
+        <v>496.5</v>
+      </c>
+    </row>
+    <row r="59" spans="1:18" ht="29" x14ac:dyDescent="0.35">
       <c r="B59" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="61" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A61" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="B61" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C61" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D61" s="3"/>
-      <c r="E61" s="3"/>
-      <c r="F61" s="3"/>
-      <c r="G61" s="3"/>
-      <c r="H61" s="3"/>
-      <c r="I61" s="3"/>
-      <c r="J61" s="3"/>
-      <c r="K61" s="3"/>
-      <c r="L61" s="3"/>
-      <c r="M61" s="3"/>
-      <c r="N61" s="3">
-        <v>0.24</v>
-      </c>
-      <c r="O61" s="3">
-        <v>13.2</v>
-      </c>
-      <c r="P61" s="3">
-        <v>285.55</v>
-      </c>
-      <c r="Q61" s="3">
-        <v>572.4</v>
-      </c>
-    </row>
-    <row r="62" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A62" s="3"/>
-      <c r="B62" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C62" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D62" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E62" s="3"/>
-      <c r="F62" s="3"/>
-      <c r="G62" s="3"/>
-      <c r="H62" s="3"/>
-      <c r="I62" s="3"/>
-      <c r="J62" s="3"/>
-      <c r="K62" s="3"/>
-      <c r="L62" s="3"/>
-      <c r="M62" s="3"/>
-      <c r="N62" s="3">
-        <v>0.19</v>
-      </c>
-      <c r="O62" s="3">
-        <v>20.399999999999999</v>
-      </c>
-      <c r="P62" s="3">
-        <v>280.37</v>
-      </c>
-      <c r="Q62" s="3">
-        <v>565.70000000000005</v>
-      </c>
-    </row>
-    <row r="63" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+      <c r="E59" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F59" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G59" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H59" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I59" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K59" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L59" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M59" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="N59" s="2">
+        <v>0.33</v>
+      </c>
+      <c r="O59" s="2">
+        <v>30.6</v>
+      </c>
+      <c r="P59" s="2">
+        <v>242.16</v>
+      </c>
+      <c r="Q59" s="2">
+        <v>500.84</v>
+      </c>
+    </row>
+    <row r="60" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+      <c r="B60" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E60" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F60" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G60" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H60" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I60" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K60" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="N60" s="2">
+        <v>0.36299999999999999</v>
+      </c>
+      <c r="O60" s="2">
+        <v>30.5</v>
+      </c>
+      <c r="P60" s="2">
+        <v>241.48</v>
+      </c>
+      <c r="Q60" s="2">
+        <v>493.28</v>
+      </c>
+    </row>
+    <row r="61" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+      <c r="B61" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G61" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H61" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I61" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K61" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="N61" s="2">
+        <v>0.36</v>
+      </c>
+      <c r="O61" s="2">
+        <v>29.9</v>
+      </c>
+      <c r="P61" s="2">
+        <v>241.6</v>
+      </c>
+      <c r="Q61" s="2">
+        <v>492.36</v>
+      </c>
+    </row>
+    <row r="62" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+      <c r="B62" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F62" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G62" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H62" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I62" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K62" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="N62" s="2">
+        <v>0.33500000000000002</v>
+      </c>
+      <c r="O62" s="2">
+        <v>29.6</v>
+      </c>
+      <c r="P62" s="2">
+        <v>241.2</v>
+      </c>
+      <c r="Q62" s="2">
+        <v>490.13</v>
+      </c>
+    </row>
+    <row r="63" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B63" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="F63" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G63" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="H63" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="J63" s="2" t="s">
-        <v>24</v>
+        <v>35</v>
+      </c>
+      <c r="I63" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="K63" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="N63" s="2">
-        <v>0.27800000000000002</v>
+        <v>0.34499999999999997</v>
       </c>
       <c r="O63" s="2">
-        <v>13.1</v>
+        <v>29.2</v>
       </c>
       <c r="P63" s="2">
-        <v>282.22000000000003</v>
+        <v>243.33</v>
       </c>
       <c r="Q63" s="2">
-        <v>568.98900000000003</v>
-      </c>
-    </row>
-    <row r="64" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+        <v>488.17</v>
+      </c>
+    </row>
+    <row r="64" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B64" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="F64" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G64" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="H64" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="M64" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="K64" s="2" t="s">
         <v>8</v>
       </c>
       <c r="N64" s="2">
-        <v>0.30299999999999999</v>
+        <v>0.32600000000000001</v>
       </c>
       <c r="O64" s="2">
-        <v>12.7</v>
+        <v>28.6</v>
       </c>
       <c r="P64" s="2">
-        <v>282.93</v>
+        <v>242.71</v>
       </c>
       <c r="Q64" s="2">
-        <v>569.64</v>
-      </c>
-    </row>
-    <row r="65" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+        <v>486.53</v>
+      </c>
+    </row>
+    <row r="65" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B65" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="F65" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G65" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="H65" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="J65" s="2" t="s">
-        <v>24</v>
+        <v>14</v>
+      </c>
+      <c r="K65" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="N65" s="2">
-        <v>0.29799999999999999</v>
+        <v>0.27100000000000002</v>
       </c>
       <c r="O65" s="2">
-        <v>12.9</v>
+        <v>27.2</v>
       </c>
       <c r="P65" s="2">
-        <v>281.83</v>
+        <v>242.45</v>
       </c>
       <c r="Q65" s="2">
-        <v>566.96810000000005</v>
-      </c>
-    </row>
-    <row r="66" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+        <v>486.54</v>
+      </c>
+      <c r="R65" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="66" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B66" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="G66" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="H66" s="2" t="s">
-        <v>9</v>
+        <v>14</v>
+      </c>
+      <c r="K66" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="N66" s="2">
-        <v>0.315</v>
+        <v>0.251</v>
       </c>
       <c r="O66" s="2">
-        <v>12.2</v>
+        <v>24.6</v>
       </c>
       <c r="P66" s="2">
-        <v>281.12</v>
+        <v>243.49</v>
       </c>
       <c r="Q66" s="2">
-        <v>565.59</v>
+        <v>488.57</v>
       </c>
     </row>
     <row r="67" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B67" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H67" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="N67" s="2">
-        <v>0.28899999999999998</v>
-      </c>
-      <c r="O67" s="2">
-        <v>10.4</v>
-      </c>
-      <c r="P67" s="2">
-        <v>283.39999999999998</v>
-      </c>
-      <c r="Q67" s="2">
-        <v>566.02</v>
-      </c>
-    </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="B68" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H68" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="N68" s="2">
-        <v>0.33700000000000002</v>
-      </c>
-      <c r="O68" s="2">
-        <v>8.2899999999999991</v>
-      </c>
-      <c r="P68" s="2">
-        <v>283.74</v>
-      </c>
-      <c r="Q68" s="2">
-        <v>566.79999999999995</v>
-      </c>
-      <c r="R68" t="s">
-        <v>8</v>
+    </row>
+    <row r="69" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A69" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B69" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C69" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D69" s="3"/>
+      <c r="E69" s="3"/>
+      <c r="F69" s="3"/>
+      <c r="G69" s="3"/>
+      <c r="H69" s="3"/>
+      <c r="I69" s="3"/>
+      <c r="J69" s="3"/>
+      <c r="K69" s="3"/>
+      <c r="L69" s="3"/>
+      <c r="M69" s="3"/>
+      <c r="N69" s="3">
+        <v>0.24</v>
+      </c>
+      <c r="O69" s="3">
+        <v>13.2</v>
+      </c>
+      <c r="P69" s="3">
+        <v>285.55</v>
+      </c>
+      <c r="Q69" s="3">
+        <v>572.4</v>
       </c>
     </row>
     <row r="70" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A70" s="3" t="s">
-        <v>25</v>
-      </c>
+      <c r="A70" s="3"/>
       <c r="B70" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C70" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="D70" s="3"/>
+      <c r="D70" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="E70" s="3"/>
       <c r="F70" s="3"/>
       <c r="G70" s="3"/>
@@ -2396,49 +2613,39 @@
       <c r="L70" s="3"/>
       <c r="M70" s="3"/>
       <c r="N70" s="3">
-        <v>0.48499999999999999</v>
+        <v>0.19</v>
       </c>
       <c r="O70" s="3">
-        <v>23.7</v>
+        <v>20.399999999999999</v>
       </c>
       <c r="P70" s="3">
-        <v>588.19000000000005</v>
+        <v>280.37</v>
       </c>
       <c r="Q70" s="3">
-        <v>1158.29</v>
-      </c>
-    </row>
-    <row r="71" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A71" s="3"/>
-      <c r="B71" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C71" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D71" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E71" s="3"/>
-      <c r="F71" s="3"/>
-      <c r="G71" s="3"/>
-      <c r="H71" s="3"/>
-      <c r="I71" s="3"/>
-      <c r="J71" s="3"/>
-      <c r="K71" s="3"/>
-      <c r="L71" s="3"/>
-      <c r="M71" s="3"/>
-      <c r="N71" s="3">
-        <v>0.40899999999999997</v>
-      </c>
-      <c r="O71" s="3">
-        <v>24</v>
-      </c>
-      <c r="P71" s="3">
-        <v>590.98</v>
-      </c>
-      <c r="Q71" s="3">
-        <v>1168.33</v>
+        <v>565.70000000000005</v>
+      </c>
+    </row>
+    <row r="71" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+      <c r="B71" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H71" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J71" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="N71" s="2">
+        <v>0.27800000000000002</v>
+      </c>
+      <c r="O71" s="2">
+        <v>13.1</v>
+      </c>
+      <c r="P71" s="2">
+        <v>282.22000000000003</v>
+      </c>
+      <c r="Q71" s="2">
+        <v>568.98900000000003</v>
       </c>
     </row>
     <row r="72" spans="1:18" ht="29" x14ac:dyDescent="0.35">
@@ -2448,20 +2655,20 @@
       <c r="H72" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="J72" s="2" t="s">
-        <v>24</v>
+      <c r="M72" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="N72" s="2">
-        <v>0.52700000000000002</v>
+        <v>0.30299999999999999</v>
       </c>
       <c r="O72" s="2">
-        <v>20.100000000000001</v>
+        <v>12.7</v>
       </c>
       <c r="P72" s="2">
-        <v>584.29</v>
+        <v>282.93</v>
       </c>
       <c r="Q72" s="2">
-        <v>1156.7</v>
+        <v>569.64</v>
       </c>
     </row>
     <row r="73" spans="1:18" ht="29" x14ac:dyDescent="0.35">
@@ -2471,20 +2678,20 @@
       <c r="H73" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="L73" s="2" t="s">
-        <v>8</v>
+      <c r="J73" s="2" t="s">
+        <v>23</v>
       </c>
       <c r="N73" s="2">
-        <v>0.29299999999999998</v>
+        <v>0.29799999999999999</v>
       </c>
       <c r="O73" s="2">
-        <v>17.8</v>
+        <v>12.9</v>
       </c>
       <c r="P73" s="2">
-        <v>587.42999999999995</v>
+        <v>281.83</v>
       </c>
       <c r="Q73" s="2">
-        <v>1165.76</v>
+        <v>566.96810000000005</v>
       </c>
     </row>
     <row r="74" spans="1:18" ht="29" x14ac:dyDescent="0.35">
@@ -2494,42 +2701,217 @@
       <c r="H74" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="J74" s="2" t="s">
+      <c r="N74" s="2">
+        <v>0.315</v>
+      </c>
+      <c r="O74" s="2">
+        <v>12.2</v>
+      </c>
+      <c r="P74" s="2">
+        <v>281.12</v>
+      </c>
+      <c r="Q74" s="2">
+        <v>565.59</v>
+      </c>
+    </row>
+    <row r="75" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="B75" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H75" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="N75" s="2">
+        <v>0.28899999999999998</v>
+      </c>
+      <c r="O75" s="2">
+        <v>10.4</v>
+      </c>
+      <c r="P75" s="2">
+        <v>283.39999999999998</v>
+      </c>
+      <c r="Q75" s="2">
+        <v>566.02</v>
+      </c>
+    </row>
+    <row r="76" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="B76" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H76" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="N76" s="2">
+        <v>0.33700000000000002</v>
+      </c>
+      <c r="O76" s="2">
+        <v>8.2899999999999991</v>
+      </c>
+      <c r="P76" s="2">
+        <v>283.74</v>
+      </c>
+      <c r="Q76" s="2">
+        <v>566.79999999999995</v>
+      </c>
+      <c r="R76" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="78" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A78" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="N74" s="2">
+      <c r="B78" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C78" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D78" s="3"/>
+      <c r="E78" s="3"/>
+      <c r="F78" s="3"/>
+      <c r="G78" s="3"/>
+      <c r="H78" s="3"/>
+      <c r="I78" s="3"/>
+      <c r="J78" s="3"/>
+      <c r="K78" s="3"/>
+      <c r="L78" s="3"/>
+      <c r="M78" s="3"/>
+      <c r="N78" s="3">
+        <v>0.48499999999999999</v>
+      </c>
+      <c r="O78" s="3">
+        <v>23.7</v>
+      </c>
+      <c r="P78" s="3">
+        <v>588.19000000000005</v>
+      </c>
+      <c r="Q78" s="3">
+        <v>1158.29</v>
+      </c>
+    </row>
+    <row r="79" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A79" s="3"/>
+      <c r="B79" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C79" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D79" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E79" s="3"/>
+      <c r="F79" s="3"/>
+      <c r="G79" s="3"/>
+      <c r="H79" s="3"/>
+      <c r="I79" s="3"/>
+      <c r="J79" s="3"/>
+      <c r="K79" s="3"/>
+      <c r="L79" s="3"/>
+      <c r="M79" s="3"/>
+      <c r="N79" s="3">
+        <v>0.40899999999999997</v>
+      </c>
+      <c r="O79" s="3">
+        <v>24</v>
+      </c>
+      <c r="P79" s="3">
+        <v>590.98</v>
+      </c>
+      <c r="Q79" s="3">
+        <v>1168.33</v>
+      </c>
+    </row>
+    <row r="80" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+      <c r="B80" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H80" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J80" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="N80" s="2">
+        <v>0.52700000000000002</v>
+      </c>
+      <c r="O80" s="2">
+        <v>20.100000000000001</v>
+      </c>
+      <c r="P80" s="2">
+        <v>584.29</v>
+      </c>
+      <c r="Q80" s="2">
+        <v>1156.7</v>
+      </c>
+    </row>
+    <row r="81" spans="2:18" ht="29" x14ac:dyDescent="0.35">
+      <c r="B81" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H81" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="L81" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="N81" s="2">
+        <v>0.29299999999999998</v>
+      </c>
+      <c r="O81" s="2">
+        <v>17.8</v>
+      </c>
+      <c r="P81" s="2">
+        <v>587.42999999999995</v>
+      </c>
+      <c r="Q81" s="2">
+        <v>1165.76</v>
+      </c>
+    </row>
+    <row r="82" spans="2:18" ht="29" x14ac:dyDescent="0.35">
+      <c r="B82" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H82" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="J82" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="N82" s="2">
         <v>0.629</v>
       </c>
-      <c r="O74" s="2">
+      <c r="O82" s="2">
         <v>18.8</v>
       </c>
-      <c r="P74" s="2">
+      <c r="P82" s="2">
         <v>583.66999999999996</v>
       </c>
-      <c r="Q74" s="2">
+      <c r="Q82" s="2">
         <v>1157.67</v>
       </c>
-      <c r="R74" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="75" spans="1:18" ht="29" x14ac:dyDescent="0.35">
-      <c r="B75" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H75" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="N75" s="2">
+      <c r="R82" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="83" spans="2:18" ht="29" x14ac:dyDescent="0.35">
+      <c r="B83" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H83" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="N83" s="2">
         <v>0.59899999999999998</v>
       </c>
-      <c r="O75" s="2">
+      <c r="O83" s="2">
         <v>16.600000000000001</v>
       </c>
-      <c r="P75" s="2">
+      <c r="P83" s="2">
         <v>584.94000000000005</v>
       </c>
-      <c r="Q75" s="2">
+      <c r="Q83" s="2">
         <v>1163.58</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Repeat model selection with revised variable list
</commit_message>
<xml_diff>
--- a/intermediate_data/ladybeetle_model_selection_results.xlsx
+++ b/intermediate_data/ladybeetle_model_selection_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cbahlai\Dropbox\Active Projects\Ohio_ladybeetles\intermediate_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CDBEB11-9A20-4870-93A7-B6F7088440A9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15C5D270-56CF-41C3-8594-C6F1426E0682}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-1650" windowWidth="29040" windowHeight="15840" xr2:uid="{6C3B7B1D-1C13-4467-BFB9-A32EE3A2C408}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="37">
   <si>
     <t>Target Species</t>
   </si>
@@ -114,9 +114,6 @@
     <t>Decade</t>
   </si>
   <si>
-    <t>Rate of landscape change</t>
-  </si>
-  <si>
     <t>Latitude</t>
   </si>
   <si>
@@ -139,6 +136,12 @@
   </si>
   <si>
     <t>Forest, Developed</t>
+  </si>
+  <si>
+    <t>Although that doesn't impove the model, there's significant concurvity issues so will try taking out a few more variables</t>
+  </si>
+  <si>
+    <t>Best model without concurvity issues</t>
   </si>
 </sst>
 </file>
@@ -514,13 +517,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF59FA38-E72D-4E06-86CB-265EAD803A1A}">
-  <dimension ref="A1:S83"/>
+  <dimension ref="A1:R85"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B50" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="B72" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="R67" sqref="R67"/>
+      <selection pane="bottomRight" activeCell="R85" sqref="R85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -532,16 +535,16 @@
     <col min="5" max="5" width="7.7265625" style="2" customWidth="1"/>
     <col min="6" max="6" width="9.36328125" style="2" customWidth="1"/>
     <col min="7" max="7" width="9.08984375" style="2" customWidth="1"/>
-    <col min="8" max="9" width="17.453125" style="2" customWidth="1"/>
-    <col min="10" max="11" width="14.08984375" style="2" customWidth="1"/>
-    <col min="12" max="12" width="8.7265625" style="2"/>
-    <col min="13" max="13" width="10.6328125" style="2" customWidth="1"/>
-    <col min="14" max="14" width="17.6328125" style="2" customWidth="1"/>
-    <col min="15" max="15" width="12.1796875" style="2" customWidth="1"/>
-    <col min="16" max="17" width="8.7265625" style="2"/>
+    <col min="8" max="8" width="17.453125" style="2" customWidth="1"/>
+    <col min="9" max="10" width="14.08984375" style="2" customWidth="1"/>
+    <col min="11" max="11" width="8.7265625" style="2"/>
+    <col min="12" max="12" width="10.6328125" style="2" customWidth="1"/>
+    <col min="13" max="13" width="17.6328125" style="2" customWidth="1"/>
+    <col min="14" max="14" width="12.1796875" style="2" customWidth="1"/>
+    <col min="15" max="16" width="8.7265625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -558,50 +561,47 @@
         <v>26</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="H1" s="1" t="s">
         <v>2</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>10</v>
+        <v>29</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="O1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="P1" s="1" t="str">
+      <c r="O1" s="1" t="str">
         <f>"-REML"</f>
         <v>-REML</v>
       </c>
+      <c r="P1" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="Q1" s="1" t="s">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.35">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
         <v>7</v>
       </c>
@@ -620,21 +620,20 @@
       <c r="J2" s="3"/>
       <c r="K2" s="3"/>
       <c r="L2" s="3"/>
-      <c r="M2" s="3"/>
+      <c r="M2" s="3">
+        <v>0.39100000000000001</v>
+      </c>
       <c r="N2" s="3">
-        <v>0.39100000000000001</v>
+        <v>10.9</v>
       </c>
       <c r="O2" s="3">
-        <v>10.9</v>
+        <v>807.7</v>
       </c>
       <c r="P2" s="3">
-        <v>807.7</v>
-      </c>
-      <c r="Q2" s="3">
         <v>1608.2</v>
       </c>
     </row>
-    <row r="3" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3"/>
       <c r="B3" s="3" t="s">
         <v>8</v>
@@ -653,21 +652,20 @@
       <c r="J3" s="3"/>
       <c r="K3" s="3"/>
       <c r="L3" s="3"/>
-      <c r="M3" s="3"/>
+      <c r="M3" s="3">
+        <v>0.38100000000000001</v>
+      </c>
       <c r="N3" s="3">
-        <v>0.38100000000000001</v>
+        <v>21.9</v>
       </c>
       <c r="O3" s="3">
-        <v>21.9</v>
+        <v>795.63</v>
       </c>
       <c r="P3" s="3">
-        <v>795.63</v>
-      </c>
-      <c r="Q3" s="3">
         <v>1585.6</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:18" ht="29" x14ac:dyDescent="0.35">
       <c r="B4" s="2" t="s">
         <v>8</v>
       </c>
@@ -684,25 +682,22 @@
         <v>9</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>8</v>
+        <v>8</v>
+      </c>
+      <c r="M4" s="2">
+        <v>0.48480000000000001</v>
       </c>
       <c r="N4" s="2">
-        <v>0.49399999999999999</v>
+        <v>15.3</v>
       </c>
       <c r="O4" s="2">
-        <v>18.7</v>
+        <v>801.94</v>
       </c>
       <c r="P4" s="2">
-        <v>796.88</v>
-      </c>
-      <c r="Q4" s="2">
-        <v>1581.79</v>
-      </c>
-    </row>
-    <row r="5" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+        <v>1590.28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" ht="29" x14ac:dyDescent="0.35">
       <c r="B5" s="2" t="s">
         <v>8</v>
       </c>
@@ -718,26 +713,23 @@
       <c r="H5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="I5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>8</v>
+      <c r="J5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M5" s="2">
+        <v>0.39900000000000002</v>
       </c>
       <c r="N5" s="2">
-        <v>0.45100000000000001</v>
+        <v>21.4</v>
       </c>
       <c r="O5" s="2">
-        <v>23.6</v>
+        <v>782.7</v>
       </c>
       <c r="P5" s="2">
-        <v>780.08</v>
-      </c>
-      <c r="Q5" s="2">
-        <v>1548.13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+        <v>1550.434</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" ht="29" x14ac:dyDescent="0.35">
       <c r="B6" s="2" t="s">
         <v>8</v>
       </c>
@@ -753,8 +745,8 @@
       <c r="H6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="I6" s="2" t="s">
-        <v>9</v>
+      <c r="J6" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>8</v>
@@ -762,30 +754,24 @@
       <c r="L6" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="M6" s="2" t="s">
-        <v>8</v>
+      <c r="M6" s="2">
+        <v>0.49399999999999999</v>
       </c>
       <c r="N6" s="2">
-        <v>0.52</v>
+        <v>21.7</v>
       </c>
       <c r="O6" s="2">
-        <v>24</v>
+        <v>783.98</v>
       </c>
       <c r="P6" s="2">
-        <v>781.27</v>
-      </c>
-      <c r="Q6" s="2">
-        <v>1549.68</v>
-      </c>
-    </row>
-    <row r="7" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+        <v>1552.7090000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" ht="29" x14ac:dyDescent="0.35">
       <c r="B7" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F7" s="2" t="s">
         <v>8</v>
       </c>
       <c r="G7" s="2" t="s">
@@ -794,29 +780,29 @@
       <c r="H7" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="I7" s="2" t="s">
-        <v>9</v>
+      <c r="J7" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="M7" s="2" t="s">
-        <v>8</v>
+      <c r="L7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M7" s="2">
+        <v>0.47899999999999998</v>
       </c>
       <c r="N7" s="2">
-        <v>0.52100000000000002</v>
+        <v>21.3</v>
       </c>
       <c r="O7" s="2">
-        <v>23.9</v>
+        <v>781.47</v>
       </c>
       <c r="P7" s="2">
-        <v>780.46</v>
-      </c>
-      <c r="Q7" s="2">
-        <v>1548.39</v>
-      </c>
-    </row>
-    <row r="8" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+        <v>1548.45</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B8" s="2" t="s">
         <v>8</v>
       </c>
@@ -827,28 +813,31 @@
         <v>8</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>9</v>
+        <v>13</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="L8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M8" s="2">
+        <v>0.47899999999999998</v>
+      </c>
       <c r="N8" s="2">
-        <v>0.46200000000000002</v>
+        <v>20.9</v>
       </c>
       <c r="O8" s="2">
-        <v>23</v>
+        <v>781.79</v>
       </c>
       <c r="P8" s="2">
-        <v>778.31</v>
-      </c>
-      <c r="Q8" s="2">
-        <v>1545.33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+        <v>1546.83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B9" s="2" t="s">
         <v>8</v>
       </c>
@@ -859,28 +848,31 @@
         <v>8</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I9" s="2" t="s">
-        <v>13</v>
+        <v>17</v>
+      </c>
+      <c r="J9" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="K9" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="L9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M9" s="2">
+        <v>0.47899999999999998</v>
+      </c>
       <c r="N9" s="2">
-        <v>0.43099999999999999</v>
+        <v>20.6</v>
       </c>
       <c r="O9" s="2">
-        <v>22.7</v>
+        <v>780.53</v>
       </c>
       <c r="P9" s="2">
-        <v>779.25</v>
-      </c>
-      <c r="Q9" s="2">
-        <v>1543.37</v>
-      </c>
-    </row>
-    <row r="10" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+        <v>1543.88</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B10" s="2" t="s">
         <v>8</v>
       </c>
@@ -891,28 +883,28 @@
         <v>8</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I10" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="K10" s="2" t="s">
-        <v>8</v>
+        <v>17</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="L10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M10" s="2">
+        <v>0.48299999999999998</v>
       </c>
       <c r="N10" s="2">
-        <v>0.45100000000000001</v>
+        <v>20.5</v>
       </c>
       <c r="O10" s="2">
-        <v>22.2</v>
+        <v>779.7</v>
       </c>
       <c r="P10" s="2">
-        <v>780.47</v>
-      </c>
-      <c r="Q10" s="2">
-        <v>1542.02</v>
-      </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.35">
+        <v>1542.24</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B11" s="2" t="s">
         <v>8</v>
       </c>
@@ -925,26 +917,26 @@
       <c r="H11" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="I11" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="K11" s="2" t="s">
-        <v>8</v>
+      <c r="J11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M11" s="2">
+        <v>0.40400000000000003</v>
       </c>
       <c r="N11" s="2">
-        <v>0.40799999999999997</v>
+        <v>20.399999999999999</v>
       </c>
       <c r="O11" s="2">
-        <v>21.7</v>
+        <v>778.87</v>
       </c>
       <c r="P11" s="2">
-        <v>779.68</v>
-      </c>
-      <c r="Q11" s="2">
-        <v>1541.04</v>
-      </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.35">
+        <v>1541.03</v>
+      </c>
+      <c r="Q11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B12" s="2" t="s">
         <v>8</v>
       </c>
@@ -954,87 +946,33 @@
       <c r="G12" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H12" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K12" s="2" t="s">
-        <v>8</v>
+      <c r="J12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M12" s="2">
+        <v>0.30099999999999999</v>
       </c>
       <c r="N12" s="2">
-        <v>0.42099999999999999</v>
+        <v>19.100000000000001</v>
       </c>
       <c r="O12" s="2">
-        <v>21.2</v>
+        <v>782.55</v>
       </c>
       <c r="P12" s="2">
-        <v>779.32</v>
-      </c>
-      <c r="Q12" s="2">
-        <v>1540.1289999999999</v>
-      </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.35">
+        <v>1551.126</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B13" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E13" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K13" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="N13" s="2">
-        <v>0.40400000000000003</v>
-      </c>
-      <c r="O13" s="2">
-        <v>20.399999999999999</v>
-      </c>
-      <c r="P13" s="2">
-        <v>778.87</v>
-      </c>
-      <c r="Q13" s="2">
-        <v>1541.03</v>
-      </c>
-      <c r="R13" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.35">
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B14" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E14" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="K14" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="N14" s="2">
-        <v>0.30099999999999999</v>
-      </c>
-      <c r="O14" s="2">
-        <v>19.100000000000001</v>
-      </c>
-      <c r="P14" s="2">
-        <v>782.55</v>
-      </c>
-      <c r="Q14" s="2">
-        <v>1551.1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="16" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>16</v>
       </c>
@@ -1053,21 +991,20 @@
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
       <c r="L16" s="3"/>
-      <c r="M16" s="3"/>
+      <c r="M16" s="3">
+        <v>0.30099999999999999</v>
+      </c>
       <c r="N16" s="3">
-        <v>0.30099999999999999</v>
+        <v>1.85</v>
       </c>
       <c r="O16" s="3">
-        <v>1.85</v>
+        <v>221.25</v>
       </c>
       <c r="P16" s="3">
-        <v>221.25</v>
-      </c>
-      <c r="Q16" s="3">
         <v>445.4</v>
       </c>
     </row>
-    <row r="17" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="3"/>
       <c r="B17" s="3" t="s">
         <v>8</v>
@@ -1086,21 +1023,20 @@
       <c r="J17" s="3"/>
       <c r="K17" s="3"/>
       <c r="L17" s="3"/>
-      <c r="M17" s="3"/>
+      <c r="M17" s="3">
+        <v>0.32800000000000001</v>
+      </c>
       <c r="N17" s="3">
-        <v>0.32800000000000001</v>
+        <v>7.92</v>
       </c>
       <c r="O17" s="3">
-        <v>7.92</v>
+        <v>217.61</v>
       </c>
       <c r="P17" s="3">
-        <v>217.61</v>
-      </c>
-      <c r="Q17" s="3">
         <v>447.3</v>
       </c>
     </row>
-    <row r="18" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:18" ht="29" x14ac:dyDescent="0.35">
       <c r="B18" s="2" t="s">
         <v>8</v>
       </c>
@@ -1117,28 +1053,25 @@
         <v>9</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="J18" s="2" t="s">
-        <v>8</v>
+        <v>8</v>
+      </c>
+      <c r="M18" s="2">
+        <v>-0.36299999999999999</v>
       </c>
       <c r="N18" s="2">
-        <v>-0.42699999999999999</v>
+        <v>31.1</v>
       </c>
       <c r="O18" s="2">
-        <v>34.4</v>
+        <v>197.62</v>
       </c>
       <c r="P18" s="2">
-        <v>194.8</v>
-      </c>
-      <c r="Q18" s="2">
-        <v>402.69</v>
-      </c>
-      <c r="S18" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="19" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+        <v>400.2</v>
+      </c>
+      <c r="R18" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" ht="29" x14ac:dyDescent="0.35">
       <c r="B19" s="2" t="s">
         <v>8</v>
       </c>
@@ -1154,26 +1087,23 @@
       <c r="H19" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="I19" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="K19" s="2" t="s">
-        <v>8</v>
+      <c r="J19" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M19" s="2">
+        <v>-0.34699999999999998</v>
       </c>
       <c r="N19" s="2">
-        <v>-0.45500000000000002</v>
+        <v>31.3</v>
       </c>
       <c r="O19" s="2">
-        <v>34.700000000000003</v>
+        <v>196.74</v>
       </c>
       <c r="P19" s="2">
-        <v>193.91</v>
-      </c>
-      <c r="Q19" s="2">
-        <v>402.57</v>
-      </c>
-    </row>
-    <row r="20" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+        <v>400.4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" ht="29" x14ac:dyDescent="0.35">
       <c r="B20" s="2" t="s">
         <v>8</v>
       </c>
@@ -1189,32 +1119,29 @@
       <c r="H20" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="I20" s="2" t="s">
-        <v>9</v>
+      <c r="J20" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="K20" s="2" t="s">
         <v>8</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="M20" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
+      </c>
+      <c r="M20" s="2">
+        <v>-0.35799999999999998</v>
       </c>
       <c r="N20" s="2">
-        <v>-0.501</v>
+        <v>31.2</v>
       </c>
       <c r="O20" s="2">
-        <v>34.700000000000003</v>
+        <v>197.54</v>
       </c>
       <c r="P20" s="2">
-        <v>194.64</v>
-      </c>
-      <c r="Q20" s="2">
-        <v>404.93</v>
-      </c>
-    </row>
-    <row r="21" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+        <v>402.72</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" ht="29" x14ac:dyDescent="0.35">
       <c r="B21" s="2" t="s">
         <v>8</v>
       </c>
@@ -1230,23 +1157,20 @@
       <c r="H21" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="I21" s="2" t="s">
-        <v>9</v>
+      <c r="M21" s="2">
+        <v>-0.38400000000000001</v>
       </c>
       <c r="N21" s="2">
-        <v>-0.502</v>
+        <v>31</v>
       </c>
       <c r="O21" s="2">
-        <v>34.5</v>
+        <v>197.04</v>
       </c>
       <c r="P21" s="2">
-        <v>194.15</v>
-      </c>
-      <c r="Q21" s="2">
-        <v>400.47</v>
-      </c>
-    </row>
-    <row r="22" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+        <v>398.44</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" ht="29" x14ac:dyDescent="0.35">
       <c r="B22" s="2" t="s">
         <v>8</v>
       </c>
@@ -1260,25 +1184,22 @@
         <v>8</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I22" s="2" t="s">
-        <v>13</v>
+        <v>19</v>
+      </c>
+      <c r="M22" s="2">
+        <v>-0.23400000000000001</v>
       </c>
       <c r="N22" s="2">
-        <v>-0.47399999999999998</v>
+        <v>30.2</v>
       </c>
       <c r="O22" s="2">
-        <v>34</v>
+        <v>199.69</v>
       </c>
       <c r="P22" s="2">
-        <v>195.96</v>
-      </c>
-      <c r="Q22" s="2">
-        <v>398.76</v>
-      </c>
-    </row>
-    <row r="23" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+        <v>396.9</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B23" s="2" t="s">
         <v>8</v>
       </c>
@@ -1292,25 +1213,25 @@
         <v>8</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I23" s="2" t="s">
-        <v>14</v>
+        <v>17</v>
+      </c>
+      <c r="M23" s="2">
+        <v>1.1769999999999999E-2</v>
       </c>
       <c r="N23" s="2">
-        <v>-0.68300000000000005</v>
+        <v>28.9</v>
       </c>
       <c r="O23" s="2">
-        <v>33.200000000000003</v>
+        <v>199.73</v>
       </c>
       <c r="P23" s="2">
-        <v>196.28</v>
-      </c>
-      <c r="Q23" s="2">
-        <v>397.51</v>
-      </c>
-    </row>
-    <row r="24" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+        <v>396.5</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B24" s="2" t="s">
         <v>8</v>
       </c>
@@ -1320,93 +1241,33 @@
       <c r="F24" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G24" s="2" t="s">
-        <v>8</v>
-      </c>
       <c r="H24" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="I24" s="2" t="s">
-        <v>14</v>
+        <v>17</v>
+      </c>
+      <c r="M24" s="2">
+        <v>0.30199999999999999</v>
       </c>
       <c r="N24" s="2">
-        <v>-0.502</v>
+        <v>23.3</v>
       </c>
       <c r="O24" s="2">
-        <v>32.6</v>
+        <v>202.51</v>
       </c>
       <c r="P24" s="2">
-        <v>198.78</v>
-      </c>
-      <c r="Q24" s="2">
-        <v>395.65</v>
-      </c>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.35">
+        <v>404.25</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B25" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E25" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F25" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G25" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H25" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I25" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="N25" s="2">
-        <v>-0.13200000000000001</v>
-      </c>
-      <c r="O25" s="2">
-        <v>31.4</v>
-      </c>
-      <c r="P25" s="2">
-        <v>198.74</v>
-      </c>
-      <c r="Q25" s="2">
-        <v>395.18</v>
-      </c>
-      <c r="R25" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.35">
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B26" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E26" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F26" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G26" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H26" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="N26" s="2">
-        <v>1.77E-2</v>
-      </c>
-      <c r="O26" s="2">
-        <v>28.9</v>
-      </c>
-      <c r="P26" s="2">
-        <v>199.73</v>
-      </c>
-      <c r="Q26" s="2">
-        <v>396.51</v>
-      </c>
-    </row>
-    <row r="28" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="28" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
         <v>18</v>
       </c>
@@ -1425,21 +1286,20 @@
       <c r="J28" s="3"/>
       <c r="K28" s="3"/>
       <c r="L28" s="3"/>
-      <c r="M28" s="3"/>
+      <c r="M28" s="3">
+        <v>0.46</v>
+      </c>
       <c r="N28" s="3">
-        <v>0.46</v>
+        <v>10.5</v>
       </c>
       <c r="O28" s="3">
-        <v>10.5</v>
+        <v>328.2</v>
       </c>
       <c r="P28" s="3">
-        <v>328.2</v>
-      </c>
-      <c r="Q28" s="3">
         <v>655.9</v>
       </c>
     </row>
-    <row r="29" spans="1:19" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A29" s="3"/>
       <c r="B29" s="3" t="s">
         <v>8</v>
@@ -1458,21 +1318,20 @@
       <c r="J29" s="3"/>
       <c r="K29" s="3"/>
       <c r="L29" s="3"/>
-      <c r="M29" s="3"/>
+      <c r="M29" s="3">
+        <v>0.53800000000000003</v>
+      </c>
       <c r="N29" s="3">
-        <v>0.53800000000000003</v>
+        <v>21</v>
       </c>
       <c r="O29" s="3">
-        <v>21</v>
+        <v>316.39</v>
       </c>
       <c r="P29" s="3">
-        <v>316.39</v>
-      </c>
-      <c r="Q29" s="3">
         <v>638.79999999999995</v>
       </c>
     </row>
-    <row r="30" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:18" ht="29" x14ac:dyDescent="0.35">
       <c r="B30" s="2" t="s">
         <v>8</v>
       </c>
@@ -1489,28 +1348,25 @@
         <v>9</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="J30" s="2" t="s">
-        <v>8</v>
+        <v>8</v>
+      </c>
+      <c r="M30" s="2">
+        <v>0.436</v>
       </c>
       <c r="N30" s="2">
-        <v>0.39800000000000002</v>
+        <v>19</v>
       </c>
       <c r="O30" s="2">
-        <v>23.5</v>
+        <v>312.32</v>
       </c>
       <c r="P30" s="2">
-        <v>308.18</v>
-      </c>
-      <c r="Q30" s="2">
-        <v>621.16999999999996</v>
-      </c>
-      <c r="S30" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="31" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+        <v>624.71</v>
+      </c>
+      <c r="R30" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" ht="29" x14ac:dyDescent="0.35">
       <c r="B31" s="2" t="s">
         <v>8</v>
       </c>
@@ -1526,26 +1382,23 @@
       <c r="H31" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="I31" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="K31" s="2" t="s">
-        <v>8</v>
+      <c r="J31" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M31" s="2">
+        <v>0.39800000000000002</v>
       </c>
       <c r="N31" s="2">
-        <v>0.36099999999999999</v>
+        <v>19.899999999999999</v>
       </c>
       <c r="O31" s="2">
-        <v>24.8</v>
+        <v>308.67</v>
       </c>
       <c r="P31" s="2">
-        <v>304.31</v>
-      </c>
-      <c r="Q31" s="2">
-        <v>616.79999999999995</v>
-      </c>
-    </row>
-    <row r="32" spans="1:19" ht="29" x14ac:dyDescent="0.35">
+        <v>621.6</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" ht="29" x14ac:dyDescent="0.35">
       <c r="B32" s="2" t="s">
         <v>8</v>
       </c>
@@ -1561,73 +1414,64 @@
       <c r="H32" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="I32" s="2" t="s">
-        <v>9</v>
+      <c r="J32" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="K32" s="2" t="s">
         <v>8</v>
       </c>
       <c r="L32" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="M32" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="M32" s="2">
+        <v>0.42299999999999999</v>
+      </c>
+      <c r="N32" s="2">
+        <v>20.2</v>
+      </c>
+      <c r="O32" s="2">
+        <v>309.69</v>
+      </c>
+      <c r="P32" s="2">
+        <v>622.79999999999995</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" ht="29" x14ac:dyDescent="0.35">
+      <c r="B33" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H33" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="N32" s="2">
-        <v>0.374</v>
-      </c>
-      <c r="O32" s="2">
-        <v>24.9</v>
-      </c>
-      <c r="P32" s="2">
-        <v>305.3</v>
-      </c>
-      <c r="Q32" s="2">
-        <v>618.5</v>
-      </c>
-    </row>
-    <row r="33" spans="1:18" ht="29" x14ac:dyDescent="0.35">
-      <c r="B33" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E33" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F33" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G33" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H33" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="I33" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="K33" s="2" t="s">
-        <v>8</v>
+      <c r="J33" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M33" s="2">
+        <v>0.38800000000000001</v>
       </c>
       <c r="N33" s="2">
-        <v>0.34200000000000003</v>
+        <v>19.8</v>
       </c>
       <c r="O33" s="2">
-        <v>24.6</v>
+        <v>309.81</v>
       </c>
       <c r="P33" s="2">
-        <v>305.60000000000002</v>
-      </c>
-      <c r="Q33" s="2">
-        <v>614.23</v>
-      </c>
-    </row>
-    <row r="34" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+        <v>618.88</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" ht="29" x14ac:dyDescent="0.35">
       <c r="B34" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E34" s="2" t="s">
-        <v>8</v>
-      </c>
       <c r="F34" s="2" t="s">
         <v>8</v>
       </c>
@@ -1635,152 +1479,92 @@
         <v>8</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="I34" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="K34" s="2" t="s">
-        <v>8</v>
+        <v>33</v>
+      </c>
+      <c r="J34" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M34" s="2">
+        <v>0.32400000000000001</v>
       </c>
       <c r="N34" s="2">
-        <v>0.313</v>
+        <v>19.100000000000001</v>
       </c>
       <c r="O34" s="2">
-        <v>24.2</v>
+        <v>308.8</v>
       </c>
       <c r="P34" s="2">
-        <v>307.11</v>
-      </c>
-      <c r="Q34" s="2">
-        <v>612.19000000000005</v>
-      </c>
-    </row>
-    <row r="35" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+        <v>617.29</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" ht="29" x14ac:dyDescent="0.35">
       <c r="B35" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F35" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G35" s="2" t="s">
-        <v>8</v>
-      </c>
       <c r="H35" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="I35" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="K35" s="2" t="s">
-        <v>8</v>
+        <v>33</v>
+      </c>
+      <c r="J35" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M35" s="2">
+        <v>0.47699999999999998</v>
       </c>
       <c r="N35" s="2">
-        <v>0.13500000000000001</v>
+        <v>17.5</v>
       </c>
       <c r="O35" s="2">
-        <v>23.5</v>
+        <v>308.64999999999998</v>
       </c>
       <c r="P35" s="2">
-        <v>306.24</v>
-      </c>
-      <c r="Q35" s="2">
-        <v>610.99</v>
-      </c>
-    </row>
-    <row r="36" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+        <v>617.85</v>
+      </c>
+      <c r="Q35" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" ht="29" x14ac:dyDescent="0.35">
       <c r="B36" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F36" s="2" t="s">
-        <v>8</v>
-      </c>
       <c r="H36" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="I36" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="K36" s="2" t="s">
-        <v>8</v>
+        <v>33</v>
+      </c>
+      <c r="J36" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M36" s="2">
+        <v>0.53200000000000003</v>
       </c>
       <c r="N36" s="2">
-        <v>0.35699999999999998</v>
+        <v>14.2</v>
       </c>
       <c r="O36" s="2">
-        <v>22</v>
+        <v>309.68</v>
       </c>
       <c r="P36" s="2">
-        <v>306.17</v>
-      </c>
-      <c r="Q36" s="2">
-        <v>611.6</v>
-      </c>
-    </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.35">
+        <v>621.83000000000004</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B37" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F37" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H37" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I37" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="K37" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="N37" s="2">
-        <v>0.35</v>
-      </c>
-      <c r="O37" s="2">
-        <v>21.5</v>
-      </c>
-      <c r="P37" s="2">
-        <v>305.64999999999998</v>
-      </c>
-      <c r="Q37" s="2">
-        <v>609.57000000000005</v>
-      </c>
-      <c r="R37" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="38" spans="1:18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B38" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="H38" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I38" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="K38" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="N38" s="2">
-        <v>0.38500000000000001</v>
-      </c>
-      <c r="O38" s="2">
-        <v>17.3</v>
-      </c>
-      <c r="P38" s="2">
-        <v>307.92</v>
-      </c>
-      <c r="Q38" s="2">
-        <v>616.82000000000005</v>
-      </c>
-    </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.35">
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B39" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="41" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A41" s="3" t="s">
         <v>21</v>
       </c>
@@ -1799,21 +1583,20 @@
       <c r="J41" s="3"/>
       <c r="K41" s="3"/>
       <c r="L41" s="3"/>
-      <c r="M41" s="3"/>
+      <c r="M41" s="3">
+        <v>0.26900000000000002</v>
+      </c>
       <c r="N41" s="3">
-        <v>0.26900000000000002</v>
+        <v>9.86</v>
       </c>
       <c r="O41" s="3">
-        <v>9.86</v>
+        <v>462.17</v>
       </c>
       <c r="P41" s="3">
-        <v>462.17</v>
-      </c>
-      <c r="Q41" s="3">
         <v>922.1</v>
       </c>
     </row>
-    <row r="42" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A42" s="3"/>
       <c r="B42" s="3" t="s">
         <v>8</v>
@@ -1832,21 +1615,20 @@
       <c r="J42" s="3"/>
       <c r="K42" s="3"/>
       <c r="L42" s="3"/>
-      <c r="M42" s="3"/>
+      <c r="M42" s="3">
+        <v>0.51400000000000001</v>
+      </c>
       <c r="N42" s="3">
-        <v>0.51400000000000001</v>
+        <v>32</v>
       </c>
       <c r="O42" s="3">
-        <v>32</v>
+        <v>450.46</v>
       </c>
       <c r="P42" s="3">
-        <v>450.46</v>
-      </c>
-      <c r="Q42" s="3">
         <v>885.6</v>
       </c>
     </row>
-    <row r="43" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:17" ht="29" x14ac:dyDescent="0.35">
       <c r="B43" s="2" t="s">
         <v>8</v>
       </c>
@@ -1863,25 +1645,22 @@
         <v>9</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="J43" s="2" t="s">
-        <v>8</v>
+        <v>8</v>
+      </c>
+      <c r="M43" s="2">
+        <v>0.625</v>
       </c>
       <c r="N43" s="2">
-        <v>0.63600000000000001</v>
+        <v>33.6</v>
       </c>
       <c r="O43" s="2">
-        <v>35.6</v>
+        <v>424.46</v>
       </c>
       <c r="P43" s="2">
-        <v>422.26</v>
-      </c>
-      <c r="Q43" s="2">
-        <v>840.36</v>
-      </c>
-    </row>
-    <row r="44" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+        <v>838.24599999999998</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" ht="29" x14ac:dyDescent="0.35">
       <c r="B44" s="2" t="s">
         <v>8</v>
       </c>
@@ -1897,26 +1676,23 @@
       <c r="H44" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="I44" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="K44" s="2" t="s">
-        <v>8</v>
+      <c r="J44" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M44" s="2">
+        <v>0.63200000000000001</v>
       </c>
       <c r="N44" s="2">
-        <v>0.64500000000000002</v>
+        <v>34.799999999999997</v>
       </c>
       <c r="O44" s="2">
-        <v>36.700000000000003</v>
+        <v>420.75</v>
       </c>
       <c r="P44" s="2">
-        <v>418.94</v>
-      </c>
-      <c r="Q44" s="2">
-        <v>836.77</v>
-      </c>
-    </row>
-    <row r="45" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+        <v>834.47</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" ht="29" x14ac:dyDescent="0.35">
       <c r="B45" s="2" t="s">
         <v>8</v>
       </c>
@@ -1932,8 +1708,8 @@
       <c r="H45" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="I45" s="2" t="s">
-        <v>9</v>
+      <c r="J45" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="K45" s="2" t="s">
         <v>8</v>
@@ -1941,23 +1717,20 @@
       <c r="L45" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="M45" s="2" t="s">
-        <v>8</v>
+      <c r="M45" s="2">
+        <v>0.19900000000000001</v>
       </c>
       <c r="N45" s="2">
-        <v>0.25800000000000001</v>
+        <v>36.799999999999997</v>
       </c>
       <c r="O45" s="2">
-        <v>38.5</v>
+        <v>417.5</v>
       </c>
       <c r="P45" s="2">
-        <v>415.96</v>
-      </c>
-      <c r="Q45" s="2">
-        <v>832.06</v>
-      </c>
-    </row>
-    <row r="46" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+        <v>829.69</v>
+      </c>
+    </row>
+    <row r="46" spans="1:17" ht="29" x14ac:dyDescent="0.35">
       <c r="B46" s="2" t="s">
         <v>8</v>
       </c>
@@ -1973,8 +1746,8 @@
       <c r="H46" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="I46" s="2" t="s">
-        <v>9</v>
+      <c r="J46" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="K46" s="2" t="s">
         <v>8</v>
@@ -1982,23 +1755,20 @@
       <c r="L46" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="M46" s="2" t="s">
-        <v>8</v>
+      <c r="M46" s="2">
+        <v>0.247</v>
       </c>
       <c r="N46" s="2">
-        <v>0.30599999999999999</v>
+        <v>35.700000000000003</v>
       </c>
       <c r="O46" s="2">
-        <v>37.6</v>
+        <v>419.17</v>
       </c>
       <c r="P46" s="2">
-        <v>418.32</v>
-      </c>
-      <c r="Q46" s="2">
-        <v>832.62</v>
-      </c>
-    </row>
-    <row r="47" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+        <v>830.65</v>
+      </c>
+    </row>
+    <row r="47" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B47" s="2" t="s">
         <v>8</v>
       </c>
@@ -2014,8 +1784,8 @@
       <c r="H47" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="I47" s="2" t="s">
-        <v>9</v>
+      <c r="J47" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="K47" s="2" t="s">
         <v>8</v>
@@ -2023,30 +1793,24 @@
       <c r="L47" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="M47" s="2" t="s">
-        <v>8</v>
+      <c r="M47" s="2">
+        <v>0.21</v>
       </c>
       <c r="N47" s="2">
-        <v>0.30499999999999999</v>
+        <v>35.4</v>
       </c>
       <c r="O47" s="2">
-        <v>37.200000000000003</v>
+        <v>418.83</v>
       </c>
       <c r="P47" s="2">
-        <v>417.73</v>
-      </c>
-      <c r="Q47" s="2">
-        <v>830.9</v>
-      </c>
-    </row>
-    <row r="48" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+        <v>828.24</v>
+      </c>
+    </row>
+    <row r="48" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B48" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F48" s="2" t="s">
         <v>8</v>
       </c>
       <c r="G48" s="2" t="s">
@@ -2055,8 +1819,8 @@
       <c r="H48" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="I48" s="2" t="s">
-        <v>34</v>
+      <c r="J48" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="K48" s="2" t="s">
         <v>8</v>
@@ -2064,23 +1828,20 @@
       <c r="L48" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="M48" s="2" t="s">
-        <v>8</v>
+      <c r="M48" s="2">
+        <v>0.30299999999999999</v>
       </c>
       <c r="N48" s="2">
-        <v>0.316</v>
+        <v>33.700000000000003</v>
       </c>
       <c r="O48" s="2">
-        <v>36.9</v>
+        <v>418.28</v>
       </c>
       <c r="P48" s="2">
-        <v>419.43</v>
-      </c>
-      <c r="Q48" s="2">
-        <v>828.98</v>
-      </c>
-    </row>
-    <row r="49" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+        <v>829.32</v>
+      </c>
+    </row>
+    <row r="49" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B49" s="2" t="s">
         <v>8</v>
       </c>
@@ -2093,46 +1854,37 @@
       <c r="H49" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="I49" s="2" t="s">
-        <v>34</v>
-      </c>
       <c r="K49" s="2" t="s">
         <v>8</v>
       </c>
       <c r="L49" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="M49" s="2" t="s">
-        <v>8</v>
+      <c r="M49" s="2">
+        <v>0.46300000000000002</v>
       </c>
       <c r="N49" s="2">
-        <v>0.38600000000000001</v>
+        <v>32.799999999999997</v>
       </c>
       <c r="O49" s="2">
-        <v>35.9</v>
+        <v>420.09</v>
       </c>
       <c r="P49" s="2">
-        <v>418.03</v>
-      </c>
-      <c r="Q49" s="2">
-        <v>827.44</v>
-      </c>
-      <c r="R49" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="50" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+        <v>829.56</v>
+      </c>
+      <c r="Q49" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="50" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B50" s="2" t="s">
         <v>8</v>
       </c>
       <c r="E50" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="G50" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="I50" s="2" t="s">
-        <v>34</v>
+      <c r="H50" s="2" t="s">
+        <v>20</v>
       </c>
       <c r="K50" s="2" t="s">
         <v>8</v>
@@ -2140,23 +1892,20 @@
       <c r="L50" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="M50" s="2" t="s">
-        <v>8</v>
+      <c r="M50" s="2">
+        <v>0.32200000000000001</v>
       </c>
       <c r="N50" s="2">
-        <v>0.27300000000000002</v>
+        <v>30</v>
       </c>
       <c r="O50" s="2">
-        <v>33.9</v>
+        <v>421.74</v>
       </c>
       <c r="P50" s="2">
-        <v>419.11</v>
-      </c>
-      <c r="Q50" s="2">
-        <v>832.07</v>
-      </c>
-    </row>
-    <row r="55" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.35">
+        <v>835.88</v>
+      </c>
+    </row>
+    <row r="55" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A55" s="3" t="s">
         <v>22</v>
       </c>
@@ -2175,21 +1924,20 @@
       <c r="J55" s="3"/>
       <c r="K55" s="3"/>
       <c r="L55" s="3"/>
-      <c r="M55" s="3"/>
+      <c r="M55" s="3">
+        <v>1.8499999999999999E-2</v>
+      </c>
       <c r="N55" s="3">
-        <v>1.8499999999999999E-2</v>
+        <v>28.6</v>
       </c>
       <c r="O55" s="3">
-        <v>28.6</v>
+        <v>248.46</v>
       </c>
       <c r="P55" s="3">
-        <v>248.46</v>
-      </c>
-      <c r="Q55" s="3">
         <v>497.3</v>
       </c>
     </row>
-    <row r="56" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:17" s="4" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A56" s="3"/>
       <c r="B56" s="3" t="s">
         <v>8</v>
@@ -2208,21 +1956,20 @@
       <c r="J56" s="3"/>
       <c r="K56" s="3"/>
       <c r="L56" s="3"/>
-      <c r="M56" s="3"/>
+      <c r="M56" s="3">
+        <v>2.6100000000000002E-2</v>
+      </c>
       <c r="N56" s="3">
-        <v>2.6100000000000002E-2</v>
+        <v>30.1</v>
       </c>
       <c r="O56" s="3">
-        <v>30.1</v>
+        <v>242.65</v>
       </c>
       <c r="P56" s="3">
-        <v>242.65</v>
-      </c>
-      <c r="Q56" s="3">
         <v>510.23</v>
       </c>
     </row>
-    <row r="57" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:17" ht="29" x14ac:dyDescent="0.35">
       <c r="B57" s="2" t="s">
         <v>8</v>
       </c>
@@ -2239,25 +1986,22 @@
         <v>9</v>
       </c>
       <c r="I57" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="J57" s="2" t="s">
-        <v>8</v>
+        <v>8</v>
+      </c>
+      <c r="M57" s="2">
+        <v>0.22</v>
       </c>
       <c r="N57" s="2">
-        <v>0.222</v>
+        <v>27.6</v>
       </c>
       <c r="O57" s="2">
-        <v>29.5</v>
+        <v>244.11</v>
       </c>
       <c r="P57" s="2">
-        <v>242.93</v>
-      </c>
-      <c r="Q57" s="2">
-        <v>498.99</v>
-      </c>
-    </row>
-    <row r="58" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+        <v>494.52</v>
+      </c>
+    </row>
+    <row r="58" spans="1:17" ht="29" x14ac:dyDescent="0.35">
       <c r="B58" s="2" t="s">
         <v>8</v>
       </c>
@@ -2273,26 +2017,23 @@
       <c r="H58" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="I58" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="K58" s="2" t="s">
-        <v>8</v>
+      <c r="J58" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M58" s="2">
+        <v>0.31</v>
       </c>
       <c r="N58" s="2">
-        <v>0.34399999999999997</v>
+        <v>29.1</v>
       </c>
       <c r="O58" s="2">
-        <v>30.6</v>
+        <v>241.33</v>
       </c>
       <c r="P58" s="2">
-        <v>240.42</v>
-      </c>
-      <c r="Q58" s="2">
-        <v>496.5</v>
-      </c>
-    </row>
-    <row r="59" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+        <v>491.33</v>
+      </c>
+    </row>
+    <row r="59" spans="1:17" ht="29" x14ac:dyDescent="0.35">
       <c r="B59" s="2" t="s">
         <v>8</v>
       </c>
@@ -2308,8 +2049,8 @@
       <c r="H59" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="I59" s="2" t="s">
-        <v>9</v>
+      <c r="J59" s="2" t="s">
+        <v>8</v>
       </c>
       <c r="K59" s="2" t="s">
         <v>8</v>
@@ -2317,27 +2058,21 @@
       <c r="L59" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="M59" s="2" t="s">
-        <v>8</v>
+      <c r="M59" s="2">
+        <v>0.3</v>
       </c>
       <c r="N59" s="2">
-        <v>0.33</v>
+        <v>29.1</v>
       </c>
       <c r="O59" s="2">
-        <v>30.6</v>
+        <v>243.02</v>
       </c>
       <c r="P59" s="2">
-        <v>242.16</v>
-      </c>
-      <c r="Q59" s="2">
-        <v>500.84</v>
-      </c>
-    </row>
-    <row r="60" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+        <v>495.51</v>
+      </c>
+    </row>
+    <row r="60" spans="1:17" ht="29" x14ac:dyDescent="0.35">
       <c r="B60" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E60" s="2" t="s">
         <v>8</v>
       </c>
       <c r="F60" s="2" t="s">
@@ -2349,32 +2084,26 @@
       <c r="H60" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="I60" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="K60" s="2" t="s">
-        <v>8</v>
+      <c r="J60" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M60" s="2">
+        <v>0.312</v>
       </c>
       <c r="N60" s="2">
-        <v>0.36299999999999999</v>
+        <v>28.8</v>
       </c>
       <c r="O60" s="2">
-        <v>30.5</v>
+        <v>240.78</v>
       </c>
       <c r="P60" s="2">
-        <v>241.48</v>
-      </c>
-      <c r="Q60" s="2">
-        <v>493.28</v>
-      </c>
-    </row>
-    <row r="61" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+        <v>489.01</v>
+      </c>
+    </row>
+    <row r="61" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B61" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E61" s="2" t="s">
-        <v>8</v>
-      </c>
       <c r="F61" s="2" t="s">
         <v>8</v>
       </c>
@@ -2382,176 +2111,95 @@
         <v>8</v>
       </c>
       <c r="H61" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I61" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J61" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M61" s="2">
+        <v>0.32600000000000001</v>
+      </c>
+      <c r="N61" s="2">
+        <v>28.6</v>
+      </c>
+      <c r="O61" s="2">
+        <v>242.71</v>
+      </c>
+      <c r="P61" s="2">
+        <v>486.52</v>
+      </c>
+    </row>
+    <row r="62" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="B62" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F62" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G62" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H62" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="K61" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="N61" s="2">
-        <v>0.36</v>
-      </c>
-      <c r="O61" s="2">
-        <v>29.9</v>
-      </c>
-      <c r="P61" s="2">
-        <v>241.6</v>
-      </c>
-      <c r="Q61" s="2">
-        <v>492.36</v>
-      </c>
-    </row>
-    <row r="62" spans="1:18" ht="29" x14ac:dyDescent="0.35">
-      <c r="B62" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F62" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G62" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H62" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="I62" s="2" t="s">
+      <c r="J62" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M62" s="2">
+        <v>0.27100000000000002</v>
+      </c>
+      <c r="N62" s="2">
+        <v>27.1</v>
+      </c>
+      <c r="O62" s="2">
+        <v>242.45</v>
+      </c>
+      <c r="P62" s="2">
+        <v>486.54</v>
+      </c>
+      <c r="Q62" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="63" spans="1:17" x14ac:dyDescent="0.35">
+      <c r="B63" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G63" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H63" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="K62" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="N62" s="2">
-        <v>0.33500000000000002</v>
-      </c>
-      <c r="O62" s="2">
-        <v>29.6</v>
-      </c>
-      <c r="P62" s="2">
-        <v>241.2</v>
-      </c>
-      <c r="Q62" s="2">
-        <v>490.13</v>
-      </c>
-    </row>
-    <row r="63" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="B63" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F63" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G63" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H63" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="I63" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K63" s="2" t="s">
-        <v>8</v>
+      <c r="J63" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M63" s="2">
+        <v>0.251</v>
       </c>
       <c r="N63" s="2">
-        <v>0.34499999999999997</v>
+        <v>24.6</v>
       </c>
       <c r="O63" s="2">
-        <v>29.2</v>
+        <v>243.49</v>
       </c>
       <c r="P63" s="2">
-        <v>243.33</v>
-      </c>
-      <c r="Q63" s="2">
-        <v>488.17</v>
-      </c>
-    </row>
-    <row r="64" spans="1:18" x14ac:dyDescent="0.35">
+        <v>488.57</v>
+      </c>
+    </row>
+    <row r="64" spans="1:17" x14ac:dyDescent="0.35">
       <c r="B64" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="F64" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G64" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H64" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="K64" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="N64" s="2">
-        <v>0.32600000000000001</v>
-      </c>
-      <c r="O64" s="2">
-        <v>28.6</v>
-      </c>
-      <c r="P64" s="2">
-        <v>242.71</v>
-      </c>
-      <c r="Q64" s="2">
-        <v>486.53</v>
       </c>
     </row>
     <row r="65" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B65" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="F65" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="G65" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H65" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K65" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="N65" s="2">
-        <v>0.27100000000000002</v>
-      </c>
-      <c r="O65" s="2">
-        <v>27.2</v>
-      </c>
-      <c r="P65" s="2">
-        <v>242.45</v>
-      </c>
-      <c r="Q65" s="2">
-        <v>486.54</v>
-      </c>
-      <c r="R65" t="s">
-        <v>8</v>
-      </c>
     </row>
     <row r="66" spans="1:18" x14ac:dyDescent="0.35">
       <c r="B66" s="2" t="s">
         <v>8</v>
-      </c>
-      <c r="G66" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H66" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="K66" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="N66" s="2">
-        <v>0.251</v>
-      </c>
-      <c r="O66" s="2">
-        <v>24.6</v>
-      </c>
-      <c r="P66" s="2">
-        <v>243.49</v>
-      </c>
-      <c r="Q66" s="2">
-        <v>488.57</v>
       </c>
     </row>
     <row r="67" spans="1:18" x14ac:dyDescent="0.35">
@@ -2578,17 +2226,16 @@
       <c r="J69" s="3"/>
       <c r="K69" s="3"/>
       <c r="L69" s="3"/>
-      <c r="M69" s="3"/>
+      <c r="M69" s="3">
+        <v>0.24</v>
+      </c>
       <c r="N69" s="3">
-        <v>0.24</v>
+        <v>13.2</v>
       </c>
       <c r="O69" s="3">
-        <v>13.2</v>
+        <v>285.55</v>
       </c>
       <c r="P69" s="3">
-        <v>285.55</v>
-      </c>
-      <c r="Q69" s="3">
         <v>572.4</v>
       </c>
     </row>
@@ -2611,17 +2258,16 @@
       <c r="J70" s="3"/>
       <c r="K70" s="3"/>
       <c r="L70" s="3"/>
-      <c r="M70" s="3"/>
+      <c r="M70" s="3">
+        <v>0.19</v>
+      </c>
       <c r="N70" s="3">
-        <v>0.19</v>
+        <v>20.399999999999999</v>
       </c>
       <c r="O70" s="3">
-        <v>20.399999999999999</v>
+        <v>280.37</v>
       </c>
       <c r="P70" s="3">
-        <v>280.37</v>
-      </c>
-      <c r="Q70" s="3">
         <v>565.70000000000005</v>
       </c>
     </row>
@@ -2629,290 +2275,406 @@
       <c r="B71" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="E71" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F71" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G71" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="H71" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="J71" s="2" t="s">
+      <c r="I71" s="2" t="s">
         <v>23</v>
       </c>
+      <c r="M71" s="2">
+        <v>0.38300000000000001</v>
+      </c>
       <c r="N71" s="2">
-        <v>0.27800000000000002</v>
+        <v>18.8</v>
       </c>
       <c r="O71" s="2">
-        <v>13.1</v>
+        <v>281.45</v>
       </c>
       <c r="P71" s="2">
-        <v>282.22000000000003</v>
-      </c>
-      <c r="Q71" s="2">
-        <v>568.98900000000003</v>
+        <v>564.77</v>
       </c>
     </row>
     <row r="72" spans="1:18" ht="29" x14ac:dyDescent="0.35">
       <c r="B72" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="E72" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F72" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G72" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="H72" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="M72" s="2" t="s">
-        <v>8</v>
+      <c r="I72" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="L72" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M72" s="2">
+        <v>0.379</v>
       </c>
       <c r="N72" s="2">
-        <v>0.30299999999999999</v>
+        <v>18.899999999999999</v>
       </c>
       <c r="O72" s="2">
-        <v>12.7</v>
+        <v>282.06</v>
       </c>
       <c r="P72" s="2">
-        <v>282.93</v>
-      </c>
-      <c r="Q72" s="2">
-        <v>569.64</v>
+        <v>566.76</v>
       </c>
     </row>
     <row r="73" spans="1:18" ht="29" x14ac:dyDescent="0.35">
       <c r="B73" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="F73" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G73" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="H73" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="J73" s="2" t="s">
+      <c r="I73" s="2" t="s">
         <v>23</v>
       </c>
+      <c r="M73" s="2">
+        <v>0.36</v>
+      </c>
       <c r="N73" s="2">
-        <v>0.29799999999999999</v>
+        <v>18.100000000000001</v>
       </c>
       <c r="O73" s="2">
-        <v>12.9</v>
+        <v>280.25</v>
       </c>
       <c r="P73" s="2">
-        <v>281.83</v>
-      </c>
-      <c r="Q73" s="2">
-        <v>566.96810000000005</v>
+        <v>563.11</v>
       </c>
     </row>
     <row r="74" spans="1:18" ht="29" x14ac:dyDescent="0.35">
       <c r="B74" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="F74" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G74" s="2" t="s">
+        <v>8</v>
+      </c>
       <c r="H74" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="M74" s="2">
+        <v>0.36699999999999999</v>
+      </c>
       <c r="N74" s="2">
+        <v>17.3</v>
+      </c>
+      <c r="O74" s="2">
+        <v>279.94</v>
+      </c>
+      <c r="P74" s="2">
+        <v>562.13</v>
+      </c>
+    </row>
+    <row r="75" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+      <c r="B75" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G75" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H75" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M75" s="2">
+        <v>0.33500000000000002</v>
+      </c>
+      <c r="N75" s="2">
+        <v>14.5</v>
+      </c>
+      <c r="O75" s="2">
+        <v>280.89999999999998</v>
+      </c>
+      <c r="P75" s="2">
+        <v>564.34</v>
+      </c>
+      <c r="R75" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="76" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+      <c r="B76" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H76" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="M76" s="2">
         <v>0.315</v>
       </c>
-      <c r="O74" s="2">
+      <c r="N76" s="2">
         <v>12.2</v>
       </c>
-      <c r="P74" s="2">
+      <c r="O76" s="2">
         <v>281.12</v>
       </c>
-      <c r="Q74" s="2">
-        <v>565.59</v>
-      </c>
-    </row>
-    <row r="75" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="B75" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H75" s="2" t="s">
+      <c r="P76" s="2">
+        <v>565.5992</v>
+      </c>
+    </row>
+    <row r="77" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="B77" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H77" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="N75" s="2">
+      <c r="M77" s="2">
         <v>0.28899999999999998</v>
       </c>
-      <c r="O75" s="2">
+      <c r="N77" s="2">
         <v>10.4</v>
       </c>
-      <c r="P75" s="2">
+      <c r="O77" s="2">
         <v>283.39999999999998</v>
       </c>
-      <c r="Q75" s="2">
-        <v>566.02</v>
-      </c>
-    </row>
-    <row r="76" spans="1:18" x14ac:dyDescent="0.35">
-      <c r="B76" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H76" s="2" t="s">
+      <c r="P77" s="2">
+        <v>566.01</v>
+      </c>
+    </row>
+    <row r="78" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="B78" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H78" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="N76" s="2">
+      <c r="M78" s="2">
         <v>0.33700000000000002</v>
       </c>
-      <c r="O76" s="2">
+      <c r="N78" s="2">
         <v>8.2899999999999991</v>
       </c>
-      <c r="P76" s="2">
+      <c r="O78" s="2">
         <v>283.74</v>
       </c>
-      <c r="Q76" s="2">
-        <v>566.79999999999995</v>
-      </c>
-      <c r="R76" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="78" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A78" s="3" t="s">
+      <c r="P78" s="2">
+        <v>566.83000000000004</v>
+      </c>
+      <c r="Q78" t="s">
+        <v>8</v>
+      </c>
+      <c r="R78" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="80" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A80" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B78" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C78" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D78" s="3"/>
-      <c r="E78" s="3"/>
-      <c r="F78" s="3"/>
-      <c r="G78" s="3"/>
-      <c r="H78" s="3"/>
-      <c r="I78" s="3"/>
-      <c r="J78" s="3"/>
-      <c r="K78" s="3"/>
-      <c r="L78" s="3"/>
-      <c r="M78" s="3"/>
-      <c r="N78" s="3">
+      <c r="B80" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C80" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D80" s="3"/>
+      <c r="E80" s="3"/>
+      <c r="F80" s="3"/>
+      <c r="G80" s="3"/>
+      <c r="H80" s="3"/>
+      <c r="I80" s="3"/>
+      <c r="J80" s="3"/>
+      <c r="K80" s="3"/>
+      <c r="L80" s="3"/>
+      <c r="M80" s="3">
         <v>0.48499999999999999</v>
       </c>
-      <c r="O78" s="3">
+      <c r="N80" s="3">
         <v>23.7</v>
       </c>
-      <c r="P78" s="3">
+      <c r="O80" s="3">
         <v>588.19000000000005</v>
       </c>
-      <c r="Q78" s="3">
+      <c r="P80" s="3">
         <v>1158.29</v>
       </c>
     </row>
-    <row r="79" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A79" s="3"/>
-      <c r="B79" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C79" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D79" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="E79" s="3"/>
-      <c r="F79" s="3"/>
-      <c r="G79" s="3"/>
-      <c r="H79" s="3"/>
-      <c r="I79" s="3"/>
-      <c r="J79" s="3"/>
-      <c r="K79" s="3"/>
-      <c r="L79" s="3"/>
-      <c r="M79" s="3"/>
-      <c r="N79" s="3">
+    <row r="81" spans="1:18" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A81" s="3"/>
+      <c r="B81" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C81" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="D81" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E81" s="3"/>
+      <c r="F81" s="3"/>
+      <c r="G81" s="3"/>
+      <c r="H81" s="3"/>
+      <c r="I81" s="3"/>
+      <c r="J81" s="3"/>
+      <c r="K81" s="3"/>
+      <c r="L81" s="3"/>
+      <c r="M81" s="3">
         <v>0.40899999999999997</v>
       </c>
-      <c r="O79" s="3">
+      <c r="N81" s="3">
         <v>24</v>
       </c>
-      <c r="P79" s="3">
+      <c r="O81" s="3">
         <v>590.98</v>
       </c>
-      <c r="Q79" s="3">
+      <c r="P81" s="3">
         <v>1168.33</v>
       </c>
     </row>
-    <row r="80" spans="1:18" ht="29" x14ac:dyDescent="0.35">
-      <c r="B80" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H80" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="J80" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="N80" s="2">
-        <v>0.52700000000000002</v>
-      </c>
-      <c r="O80" s="2">
-        <v>20.100000000000001</v>
-      </c>
-      <c r="P80" s="2">
-        <v>584.29</v>
-      </c>
-      <c r="Q80" s="2">
-        <v>1156.7</v>
-      </c>
-    </row>
-    <row r="81" spans="2:18" ht="29" x14ac:dyDescent="0.35">
-      <c r="B81" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="H81" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="L81" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="N81" s="2">
-        <v>0.29299999999999998</v>
-      </c>
-      <c r="O81" s="2">
-        <v>17.8</v>
-      </c>
-      <c r="P81" s="2">
-        <v>587.42999999999995</v>
-      </c>
-      <c r="Q81" s="2">
-        <v>1165.76</v>
-      </c>
-    </row>
-    <row r="82" spans="2:18" ht="29" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:18" ht="29" x14ac:dyDescent="0.35">
       <c r="B82" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E82" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F82" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G82" s="2" t="s">
         <v>8</v>
       </c>
       <c r="H82" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="J82" s="2" t="s">
+      <c r="I82" s="2" t="s">
         <v>23</v>
       </c>
+      <c r="M82" s="2">
+        <v>0.54800000000000004</v>
+      </c>
       <c r="N82" s="2">
-        <v>0.629</v>
+        <v>28.6</v>
       </c>
       <c r="O82" s="2">
-        <v>18.8</v>
+        <v>573.02</v>
       </c>
       <c r="P82" s="2">
-        <v>583.66999999999996</v>
-      </c>
-      <c r="Q82" s="2">
-        <v>1157.67</v>
-      </c>
-      <c r="R82" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="83" spans="2:18" ht="29" x14ac:dyDescent="0.35">
+        <v>1128.71</v>
+      </c>
+    </row>
+    <row r="83" spans="1:18" ht="29" x14ac:dyDescent="0.35">
       <c r="B83" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E83" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="F83" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G83" s="2" t="s">
         <v>8</v>
       </c>
       <c r="H83" s="2" t="s">
         <v>9</v>
       </c>
+      <c r="I83" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K83" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="M83" s="2">
+        <v>0.67500000000000004</v>
+      </c>
       <c r="N83" s="2">
-        <v>0.59899999999999998</v>
+        <v>28.9</v>
       </c>
       <c r="O83" s="2">
-        <v>16.600000000000001</v>
+        <v>573.63</v>
       </c>
       <c r="P83" s="2">
-        <v>584.94000000000005</v>
-      </c>
-      <c r="Q83" s="2">
-        <v>1163.58</v>
+        <v>1129.663</v>
+      </c>
+    </row>
+    <row r="84" spans="1:18" ht="29" x14ac:dyDescent="0.35">
+      <c r="B84" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E84" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G84" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H84" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="I84" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="M84" s="2">
+        <v>0.50700000000000001</v>
+      </c>
+      <c r="N84" s="2">
+        <v>26.9</v>
+      </c>
+      <c r="O84" s="2">
+        <v>572.11</v>
+      </c>
+      <c r="P84" s="2">
+        <v>1129.97</v>
+      </c>
+    </row>
+    <row r="85" spans="1:18" x14ac:dyDescent="0.35">
+      <c r="B85" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E85" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G85" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="H85" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="I85" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="M85" s="2">
+        <v>0.46100000000000002</v>
+      </c>
+      <c r="N85" s="2">
+        <v>25.4</v>
+      </c>
+      <c r="O85" s="2">
+        <v>574.66999999999996</v>
+      </c>
+      <c r="P85" s="2">
+        <v>1132.45</v>
+      </c>
+      <c r="R85" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update model selection results file
</commit_message>
<xml_diff>
--- a/intermediate_data/ladybeetle_model_selection_results.xlsx
+++ b/intermediate_data/ladybeetle_model_selection_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cbahlai\Dropbox\Active Projects\Ohio_ladybeetles\intermediate_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FC18C6F-8440-4EBA-A4DD-DE40F21F8CB7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF1789CE-FF07-48FC-AE10-D9BB714D2987}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-1995" windowWidth="29040" windowHeight="15840" xr2:uid="{6C3B7B1D-1C13-4467-BFB9-A32EE3A2C408}"/>
   </bookViews>
@@ -523,15 +523,15 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="A82" sqref="A82:XFD82"/>
+      <selection pane="bottomRight" activeCell="R85" sqref="A1:R85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16.6328125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="20.6328125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="15.7265625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="20.26953125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="8.36328125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="6.453125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="6.6328125" style="2" customWidth="1"/>
     <col min="5" max="5" width="7.7265625" style="2" customWidth="1"/>
     <col min="6" max="6" width="9.36328125" style="2" customWidth="1"/>
     <col min="7" max="7" width="9.08984375" style="2" customWidth="1"/>

</xml_diff>